<commit_message>
Added Dash dashboard to urban mobility analysis, updated HTML to include dashboard
</commit_message>
<xml_diff>
--- a/disruptions.xlsx
+++ b/disruptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z56"/>
+  <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,17 +573,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TIMS-206062</t>
+          <t>TIMS-206167</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206062</t>
+          <t>/Road/All/Disruption/TIMS-206167</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[-0.301241,51.374535]</t>
+          <t>[-0.20651,51.58838]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -596,47 +596,48 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Works</t>
+          <t>Collisions</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>TfL works</t>
+          <t>Vehicle collision</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[A3] Hook Rise South (Westbound) at the junction of [A243] Hook Road - Lane one (of two) is closed due to works.</t>
+          <t>[A406] North Circular Road (Westbound) at the junction of [A1] Great North Way - There are lane restrictions due to a collision at this location</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Westbound traffic is slow on approach to the works with queues back to the junction with Tolworth Junction. Expect delays.</t>
+          <t xml:space="preserve">Use caution on approach and expect serious delays, traffic currently is back to East End Road
+</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-01-22T19:18:53Z</t>
+          <t>2025-01-22T19:56:36Z</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>['a3']</t>
+          <t>['a406']</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2025-01-20T08:18:22Z</t>
+          <t>2025-01-22T18:48:30Z</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2025-01-20T23:59:59Z</t>
+          <t>2025-01-22T23:59:59Z</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2025-01-22T19:18:53Z</t>
+          <t>2025-01-22T19:58:06Z</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -646,7 +647,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>[A3] HOOK RISE SOUTH (KT6,KT9) (Kingston upon Thames)</t>
+          <t>[A406] NORTH CIRCULAR ROAD (N3,NW11,NW4) (Barnet)</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -656,7 +657,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.301241, 51.374535], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.20651, 51.58838], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T2" t="b">
@@ -691,17 +692,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TIMS-206167</t>
+          <t>TIMS-204991</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206167</t>
+          <t>/Road/All/Disruption/TIMS-204991</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[-0.20651,51.58838]</t>
+          <t>[-0.130857,51.527321]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -714,48 +715,47 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Collisions</t>
+          <t>Works</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Vehicle collision</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[A406] North Circular Road (Westbound) at the junction of [A1] Great North Way - There are lane restrictions due to a collision at this location</t>
+          <t>[A501] Euston Road (Both directions) at the junction of [A4200] Upper Woburn Place - TfL drainage works - starts Upper Woburn Place, with temporary signals and will then progress onto Euston Road with lane restrictions to Gower Street.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Use caution on approach and expect serious delays, traffic currently is back to East End Road
-</t>
+          <t>Traffic is slow on approach. Expect delays.</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-01-22T19:56:36Z</t>
+          <t>2025-01-22T18:47:15Z</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>['a406']</t>
+          <t>['inner ring']</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2025-01-22T18:48:30Z</t>
+          <t>2025-01-06T11:00:00Z</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2025-01-22T23:59:59Z</t>
+          <t>2025-02-27T18:00:00Z</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>2025-01-22T19:58:06Z</t>
+          <t>2025-01-22T18:50:46Z</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -765,7 +765,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>[A406] NORTH CIRCULAR ROAD (N3,NW11,NW4) (Barnet)</t>
+          <t>[A501] EUSTON ROAD (N1C,NW1,WC1H) (Camden)</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -775,7 +775,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.20651, 51.58838], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.130857, 51.527321], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T3" t="b">
@@ -810,22 +810,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TIMS-204991</t>
+          <t>TIMS-205967</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204991</t>
+          <t>/Road/All/Disruption/TIMS-205967</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[-0.130857,51.527321]</t>
+          <t>[-0.028898,51.515905]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Serious</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -843,37 +843,37 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>[A501] Euston Road (Both directions) at the junction of [A4200] Upper Woburn Place - TfL drainage works - starts Upper Woburn Place, with temporary signals and will then progress onto Euston Road with lane restrictions to Gower Street.</t>
+          <t>[A1205] Burdett Road (Both directions) between Thomas Road and Agnes Street - A contraflow is in place due to Thames Water works.</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Traffic is slow on approach. Expect delays.</t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-01-22T18:47:15Z</t>
+          <t>2025-01-22T14:05:31Z</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>['inner ring']</t>
+          <t>['a12', 'a13']</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2025-01-06T11:00:00Z</t>
+          <t>2025-01-16T17:43:00Z</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2025-02-27T18:00:00Z</t>
+          <t>2025-03-16T23:59:00Z</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>2025-01-22T18:50:46Z</t>
+          <t>2025-01-22T14:05:31Z</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>[A501] EUSTON ROAD (N1C,NW1,WC1H) (Camden)</t>
+          <t>[A1205] BURDETT ROAD (E14,E3) (Tower Hamlets)</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -893,7 +893,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.130857, 51.527321], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.028898, 51.515905], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T4" t="b">
@@ -928,17 +928,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TIMS-205967</t>
+          <t>TIMS-204970</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205967</t>
+          <t>/Road/All/Disruption/TIMS-204970</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[-0.028898,51.515905]</t>
+          <t>[0.009195,51.515695]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -956,42 +956,42 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>TfL works</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[A1205] Burdett Road (Both directions) between Thomas Road and Agnes Street - A contraflow is in place due to Thames Water works.</t>
+          <t>Canning Town Flyover Refurbishment Works - [A13] Newham Way (Both directions) between [A13] East India Dock Road and Beckton Road - Lane closures and restrictions in place for flyover refurbishment works. Thursday 23 January two lanes closed in both directions (2200-0600) Friday 24 and Saturday 25 January, East India Dock Tunnel, closed eastbound between 21:00 and 08:00 each night and A13 reduced to one lane westbound.</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t xml:space="preserve">Traffic is flowing well. </t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-01-22T14:05:31Z</t>
+          <t>2025-01-22T19:47:42Z</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>['a12', 'a13']</t>
+          <t>['a13']</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2025-01-16T17:43:00Z</t>
+          <t>2024-12-19T08:30:00Z</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2025-03-16T23:59:00Z</t>
+          <t>2025-05-25T22:59:00Z</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>2025-01-22T14:05:31Z</t>
+          <t>2025-01-22T19:47:42Z</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>[A1205] BURDETT ROAD (E14,E3) (Tower Hamlets)</t>
+          <t>[A13] NEWHAM WAY (E16) (Newham)</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.028898, 51.515905], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [0.009195, 51.515695], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T5" t="b">
@@ -1035,8 +1035,16 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>{'type': 'Polygon', 'coordinates': [[[-0.0028763086, 51.5099584741], [-0.0027962352, 51.5097513783], [-0.002572313, 51.5095905628], [-0.0021977037, 51.5095086712], [-0.0018619051, 51.5095471286], [-0.0016297109, 51.5096506164], [-0.0013359974, 51.5098826766], [-0.0003111049, 51.5103853589], [0.000356251, 51.5108350877], [0.0008001745, 51.5112782287], [0.0011767731, 51.5117892099], [0.0016418464, 51.5127336654], [0.0016403157, 51.5130222399], [0.0019649041, 51.5133807145], [0.0026484532, 51.5138608548], [0.0027673384, 51.5139954264], [0.0028066137, 51.514147121], [0.0027731662, 51.5142773413], [0.0026598819, 51.5144137813], [0.002508688, 51.5145059431], [0.0023211254, 51.5145667524], [0.0021133473, 51.5145909719], [0.0017394762, 51.5145357248], [0.0015711803, 51.5144559326], [0.0008052751, 51.5139168934], [0.0003044024, 51.5133593979], [2.25608e-05, 51.5128714003], [1.03922e-05, 51.5127274568], [6.70903e-05, 51.5125954973], [-8.242e-06, 51.5124082845], [-0.0002380436, 51.512004943], [-0.0006611232, 51.511494134], [-0.0012732415, 51.5110545116], [-0.0022900527, 51.5105579939], [-0.002524349, 51.5104076433], [-0.002806373, 51.5101505073], [-0.0028763086, 51.5099584741]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A1261] EAST INDIA DOCK ROAD TUNNEL (E14)', 'closure': 'Open', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.000266,51.511625],[-0.000322,51.511028]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.000941,51.512837],[0.000419,51.51182]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.000726,51.512776],[0.000826,51.512945]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.000419,51.51182],[0.000266,51.511625]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.001257,51.51048],[-0.002156,51.509957]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.000945,51.510638],[-0.001257,51.51048]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.000826,51.512945],[0.002086,51.514142]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.000322,51.511028],[-0.000945,51.510638]]', 'sourceSystemId': 0}], 'sourceSystemId': 204970, 'sourceSystemKey': 'TIMS'}]</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1046,17 +1054,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TIMS-204970</t>
+          <t>TIMS-206094</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204970</t>
+          <t>/Road/All/Disruption/TIMS-206094</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[0.009195,51.515695]</t>
+          <t>[-0.202906,51.456673]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1074,42 +1082,42 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>TfL works</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Canning Town Flyover Refurbishment Works - [A13] Newham Way (Both directions) between [A13] East India Dock Road and Beckton Road - Lane closures and restrictions in place for flyover refurbishment works. Thursday 23 January two lanes closed in both directions (2200-0600) Friday 24 and Saturday 25 January, East India Dock Tunnel, closed eastbound between 21:00 and 08:00 each night and A13 reduced to one lane westbound.</t>
+          <t>[A3] West Hill (All directions) at the junction of [A205] Upper Richmond Road - Temporary signals in operation to facilitate repairs to a burst water main.</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traffic is flowing well. </t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-01-22T19:47:42Z</t>
+          <t>2025-01-22T19:13:05Z</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>['a13']</t>
+          <t>['a205', 'a3']</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2024-12-19T08:30:00Z</t>
+          <t>2025-01-20T19:20:00Z</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>2025-05-25T22:59:00Z</t>
+          <t>2025-01-25T23:59:00Z</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>2025-01-22T19:47:42Z</t>
+          <t>2025-01-22T19:13:31Z</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -1119,7 +1127,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>[A13] NEWHAM WAY (E16) (Newham)</t>
+          <t>[A3] WEST HILL (SW15,SW18) (Wandsworth)</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1129,7 +1137,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [0.009195, 51.515695], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.202906, 51.456673], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T6" t="b">
@@ -1153,16 +1161,8 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>{'type': 'Polygon', 'coordinates': [[[-0.0028763086, 51.5099584741], [-0.0027962352, 51.5097513783], [-0.002572313, 51.5095905628], [-0.0021977037, 51.5095086712], [-0.0018619051, 51.5095471286], [-0.0016297109, 51.5096506164], [-0.0013359974, 51.5098826766], [-0.0003111049, 51.5103853589], [0.000356251, 51.5108350877], [0.0008001745, 51.5112782287], [0.0011767731, 51.5117892099], [0.0016418464, 51.5127336654], [0.0016403157, 51.5130222399], [0.0019649041, 51.5133807145], [0.0026484532, 51.5138608548], [0.0027673384, 51.5139954264], [0.0028066137, 51.514147121], [0.0027731662, 51.5142773413], [0.0026598819, 51.5144137813], [0.002508688, 51.5145059431], [0.0023211254, 51.5145667524], [0.0021133473, 51.5145909719], [0.0017394762, 51.5145357248], [0.0015711803, 51.5144559326], [0.0008052751, 51.5139168934], [0.0003044024, 51.5133593979], [2.25608e-05, 51.5128714003], [1.03922e-05, 51.5127274568], [6.70903e-05, 51.5125954973], [-8.242e-06, 51.5124082845], [-0.0002380436, 51.512004943], [-0.0006611232, 51.511494134], [-0.0012732415, 51.5110545116], [-0.0022900527, 51.5105579939], [-0.002524349, 51.5104076433], [-0.002806373, 51.5101505073], [-0.0028763086, 51.5099584741]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A1261] EAST INDIA DOCK ROAD TUNNEL (E14)', 'closure': 'Open', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.000266,51.511625],[-0.000322,51.511028]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.000941,51.512837],[0.000419,51.51182]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.000726,51.512776],[0.000826,51.512945]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.000419,51.51182],[0.000266,51.511625]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.001257,51.51048],[-0.002156,51.509957]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.000945,51.510638],[-0.001257,51.51048]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.000826,51.512945],[0.002086,51.514142]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.000322,51.511028],[-0.000945,51.510638]]', 'sourceSystemId': 0}], 'sourceSystemId': 204970, 'sourceSystemKey': 'TIMS'}]</t>
-        </is>
-      </c>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1172,17 +1172,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TIMS-206094</t>
+          <t>TIMS-206066</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206094</t>
+          <t>/Road/All/Disruption/TIMS-206066</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[-0.202906,51.456673]</t>
+          <t>[-0.277053,51.375776]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1195,47 +1195,47 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Works</t>
+          <t>Asset issues</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>Traffic signal fault</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>[A3] West Hill (All directions) at the junction of [A205] Upper Richmond Road - Temporary signals in operation to facilitate repairs to a burst water main.</t>
+          <t>[A240] Kingston Road (All approaches) at the junction of Jubilee Way - Temporary traffic signals are in place due to vandalism on the ULEZ camera network.</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Traffic is flowing well.</t>
+          <t xml:space="preserve">Traffic is flowing well. </t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-01-22T19:13:05Z</t>
+          <t>2025-01-22T19:07:16Z</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>['a205', 'a3']</t>
+          <t>['a3']</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2025-01-20T19:20:00Z</t>
+          <t>2025-01-20T09:05:02Z</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>2025-01-25T23:59:00Z</t>
+          <t>2025-01-20T23:59:59Z</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>2025-01-22T19:13:31Z</t>
+          <t>2025-01-22T19:07:39Z</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>[A3] WEST HILL (SW15,SW18) (Wandsworth)</t>
+          <t>[A240] KINGSTON ROAD (KT19,KT4,KT5,KT9) (Kingston upon Thames,UNK)</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.202906, 51.456673], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.277053, 51.375776], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T7" t="b">
@@ -1290,17 +1290,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TIMS-206066</t>
+          <t>TIMS-206062</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206066</t>
+          <t>/Road/All/Disruption/TIMS-206062</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[-0.277053,51.375776]</t>
+          <t>[-0.301241,51.374535]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1313,27 +1313,27 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Asset issues</t>
+          <t>Works</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Traffic signal fault</t>
+          <t>TfL works</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>[A240] Kingston Road (All approaches) at the junction of Jubilee Way - Temporary traffic signals are in place due to vandalism on the ULEZ camera network.</t>
+          <t>[A3] Hook Rise South (Westbound) at the junction of [A243] Hook Road - Lane one (of two) is closed due to works.</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traffic is flowing well. </t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-01-22T19:07:16Z</t>
+          <t>2025-01-22T20:19:40Z</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2025-01-20T09:05:02Z</t>
+          <t>2025-01-20T08:18:22Z</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>2025-01-22T19:07:39Z</t>
+          <t>2025-01-22T20:19:40Z</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>[A240] KINGSTON ROAD (KT19,KT4,KT5,KT9) (Kingston upon Thames,UNK)</t>
+          <t>[A3] HOOK RISE SOUTH (KT6,KT9) (Kingston upon Thames)</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1373,7 +1373,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.277053, 51.375776], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.301241, 51.374535], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T8" t="b">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>2025-01-22T20:03:12Z</t>
+          <t>2025-01-22T20:12:57Z</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -3007,17 +3007,17 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>[A12] Blackwall Tunnel Northern Approach (Eastbound) at the junction of [A11] Bow Road - The roundabout is restricted by a broken down car.</t>
+          <t>[A12] Blackwall Tunnel Northern Approach (Eastbound) at the junction of [A11] Bow Road - The roundabout is blocked due to a broken down car</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Approach with caution.</t>
+          <t>Use other route.</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-01-22T20:01:11Z</t>
+          <t>2025-01-22T20:12:43Z</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>2025-01-22T20:05:17Z</t>
+          <t>2025-01-22T20:12:43Z</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -3446,17 +3446,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>TIMS-206084</t>
+          <t>TIMS-204983</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206084</t>
+          <t>/Road/All/Disruption/TIMS-204983</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>[-0.297428,51.465248]</t>
+          <t>[-0.330213,51.455737]</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -3474,22 +3474,22 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>TfL works</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>[A316] Lower Mortlake Road (Westbound) at the junction of Salisbury Road - Lane one of two is closed to facilitate Cadent Gas works.</t>
+          <t xml:space="preserve">[A316] Chertsey Road (Both directions) at the junction of [A310] London Road - There are lane restrictions in place due to junction improvement works. </t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Traffic is flowing well.</t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-01-22T19:08:26Z</t>
+          <t>2025-01-22T09:35:19Z</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -3499,17 +3499,17 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>2025-01-20T15:26:00Z</t>
+          <t>2024-12-19T10:00:00Z</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>2025-01-24T23:59:00Z</t>
+          <t>2025-07-25T04:00:00Z</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>2025-01-22T19:08:26Z</t>
+          <t>2025-01-22T09:35:32Z</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -3519,7 +3519,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>[A316] LOWER MORTLAKE ROAD (TW9) (Richmond upon Thames)</t>
+          <t>[A316] CHERTSEY ROAD (TW1,TW2) (Richmond upon Thames)</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -3529,7 +3529,7 @@
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.297428, 51.465248], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.330213, 51.455737], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T26" t="b">
@@ -3564,17 +3564,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>TIMS-204983</t>
+          <t>TIMS-206084</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204983</t>
+          <t>/Road/All/Disruption/TIMS-206084</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>[-0.330213,51.455737]</t>
+          <t>[-0.297428,51.465248]</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -3592,22 +3592,22 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>TfL works</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t xml:space="preserve">[A316] Chertsey Road (Both directions) at the junction of [A310] London Road - There are lane restrictions in place due to junction improvement works. </t>
+          <t>[A316] Lower Mortlake Road (Westbound) at the junction of Salisbury Road - Lane one of two is closed to facilitate Cadent Gas works.</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-01-22T09:35:19Z</t>
+          <t>2025-01-22T19:08:26Z</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -3617,17 +3617,17 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>2024-12-19T10:00:00Z</t>
+          <t>2025-01-20T15:26:00Z</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>2025-07-25T04:00:00Z</t>
+          <t>2025-01-24T23:59:00Z</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>2025-01-22T09:35:32Z</t>
+          <t>2025-01-22T19:08:26Z</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>[A316] CHERTSEY ROAD (TW1,TW2) (Richmond upon Thames)</t>
+          <t>[A316] LOWER MORTLAKE ROAD (TW9) (Richmond upon Thames)</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -3647,7 +3647,7 @@
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.330213, 51.455737], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.297428, 51.465248], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T27" t="b">
@@ -4044,17 +4044,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>TIMS-205753</t>
+          <t>TIMS-206121</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205753</t>
+          <t>/Road/All/Disruption/TIMS-206121</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[-0.077317,51.453151]</t>
+          <t>[-0.219026,51.55979]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -4077,7 +4077,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t xml:space="preserve">[A2216] Lordship Lane (All directions) at the junction of Heber Road - Temporary traffic signals are in operation to facilitate Thames Water works. </t>
+          <t xml:space="preserve">[A5] Cricklewood Broadway (All directions) at the junction of Mora Road - Temporary traffic signals are in operation to facilitate Thames Water works. </t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -4087,7 +4087,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-01-22T09:33:22Z</t>
+          <t>2025-01-22T08:26:09Z</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -4097,17 +4097,17 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>2025-01-18T10:00:00Z</t>
+          <t>2025-01-21T15:16:00Z</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>2025-01-28T18:00:00Z</t>
+          <t>2025-01-24T17:00:00Z</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>2025-01-22T09:33:32Z</t>
+          <t>2025-01-22T08:27:47Z</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>[A2216] LORDSHIP LANE (SE22) (Southwark)</t>
+          <t>[A5] CRICKLEWOOD BROADWAY (NW2) (Barnet,Brent)</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -4127,7 +4127,7 @@
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.077317, 51.453151], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.219026, 51.55979], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T31" t="b">
@@ -4162,17 +4162,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>TIMS-206055</t>
+          <t>TIMS-206104</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206055</t>
+          <t>/Road/All/Disruption/TIMS-206104</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>[-0.052654,51.55242]</t>
+          <t>[-0.144053,51.339619]</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -4195,17 +4195,17 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t xml:space="preserve">[A107] Lower Clapton Road (Both directions) at the junction of Powerscroft Road - Temporary traffic signals are in operation to facilitate UKPN works.   </t>
+          <t>[A2022] Little Woodcote Lane (All approaches) at the junction of [A2022] Foxley Lane - Temporary signals in place due to emergency SGN gas works.</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traffic is flowing well. </t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-01-22T18:30:19Z</t>
+          <t>2025-01-22T19:11:40Z</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -4215,17 +4215,17 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>2025-01-19T06:00:00Z</t>
+          <t>2025-01-21T09:00:00Z</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>2025-01-24T23:00:00Z</t>
+          <t>2025-02-10T21:00:00Z</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>2025-01-22T18:30:19Z</t>
+          <t>2025-01-22T19:11:40Z</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -4235,7 +4235,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>[A107] LOWER CLAPTON ROAD (E5,E8,E9) (Hackney)</t>
+          <t>[A2022] LITTLE WOODCOTE LANE (CR8,SM5) (Croydon,Sutton)</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -4245,7 +4245,7 @@
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.052654, 51.55242], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.144053, 51.339619], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T32" t="b">
@@ -4280,17 +4280,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>TIMS-206054</t>
+          <t>TIMS-205753</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206054</t>
+          <t>/Road/All/Disruption/TIMS-205753</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>[-0.12737,51.509315]</t>
+          <t>[-0.077317,51.453151]</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -4313,17 +4313,17 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>[A400] St Martins Place (All directions) at the junction of [A400] Charing Cross Road - Temporary signals in operation to facilitate Cadent Gas works.</t>
+          <t xml:space="preserve">[A2216] Lordship Lane (All directions) at the junction of Heber Road - Temporary traffic signals are in operation to facilitate Thames Water works. </t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Traffic is flowing well.</t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-01-22T17:51:14Z</t>
+          <t>2025-01-22T09:33:22Z</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -4333,17 +4333,17 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>2025-01-19T17:45:00Z</t>
+          <t>2025-01-18T10:00:00Z</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>2025-01-24T17:00:00Z</t>
+          <t>2025-01-28T18:00:00Z</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>2025-01-22T17:51:14Z</t>
+          <t>2025-01-22T09:33:32Z</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>[A400] ST MARTINS PLACE (WC2N) (Westminster)</t>
+          <t>[A2216] LORDSHIP LANE (SE22) (Southwark)</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -4363,7 +4363,7 @@
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.12737, 51.509315], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.077317, 51.453151], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T33" t="b">
@@ -4398,17 +4398,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>TIMS-206104</t>
+          <t>TIMS-206055</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206104</t>
+          <t>/Road/All/Disruption/TIMS-206055</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[-0.144053,51.339619]</t>
+          <t>[-0.052654,51.55242]</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -4431,17 +4431,17 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>[A2022] Little Woodcote Lane (All approaches) at the junction of [A2022] Foxley Lane - Temporary signals in place due to emergency SGN gas works.</t>
+          <t xml:space="preserve">[A107] Lower Clapton Road (Both directions) at the junction of Powerscroft Road - Temporary traffic signals are in operation to facilitate UKPN works.   </t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Traffic is flowing well.</t>
+          <t xml:space="preserve">Traffic is flowing well. </t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-01-22T19:11:40Z</t>
+          <t>2025-01-22T18:30:19Z</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -4451,17 +4451,17 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>2025-01-21T09:00:00Z</t>
+          <t>2025-01-19T06:00:00Z</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>2025-02-10T21:00:00Z</t>
+          <t>2025-01-24T23:00:00Z</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>2025-01-22T19:11:40Z</t>
+          <t>2025-01-22T18:30:19Z</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -4471,7 +4471,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>[A2022] LITTLE WOODCOTE LANE (CR8,SM5) (Croydon,Sutton)</t>
+          <t>[A107] LOWER CLAPTON ROAD (E5,E8,E9) (Hackney)</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.144053, 51.339619], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.052654, 51.55242], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T34" t="b">
@@ -4516,17 +4516,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>TIMS-206121</t>
+          <t>TIMS-206069</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206121</t>
+          <t>/Road/All/Disruption/TIMS-206069</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>[-0.219026,51.55979]</t>
+          <t>[-0.156729,51.49289]</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -4549,17 +4549,17 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t xml:space="preserve">[A5] Cricklewood Broadway (All directions) at the junction of Mora Road - Temporary traffic signals are in operation to facilitate Thames Water works. </t>
+          <t>[A3216] Sloane Square (Eastbound) at the junction of Sedding Street - Road is closed due to emergency Thames Water and Cadent Gas works</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t>Use an alternative route. There are no reported delays on diversion.</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-01-22T08:26:09Z</t>
+          <t>2025-01-22T17:51:06Z</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -4569,17 +4569,17 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>2025-01-21T15:16:00Z</t>
+          <t>2025-01-20T10:00:00Z</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>2025-01-24T17:00:00Z</t>
+          <t>2025-01-25T18:00:00Z</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>2025-01-22T08:27:47Z</t>
+          <t>2025-01-22T18:50:15Z</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -4589,7 +4589,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>[A5] CRICKLEWOOD BROADWAY (NW2) (Barnet,Brent)</t>
+          <t>[A3216] SLOANE SQUARE (SW1W,SW1X,SW3) (Kensington &amp; Chelsea,Westminster)</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -4599,7 +4599,7 @@
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.219026, 51.55979], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.156729, 51.49289], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T35" t="b">
@@ -4623,8 +4623,16 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y35" t="inlineStr"/>
-      <c r="Z35" t="inlineStr"/>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>{'type': 'Polygon', 'coordinates': [[[-0.1584777328, 51.4926860385], [-0.1584390066, 51.4925397983], [-0.1583261769, 51.4924093762], [-0.1581841856, 51.4923230989], [-0.1579722888, 51.4922562091], [-0.1576578673, 51.4922401505], [-0.1567956082, 51.4923397904], [-0.1558023405, 51.4927240695], [-0.1554594231, 51.4928949283], [-0.1552773642, 51.4931060012], [-0.1552950424, 51.4933454702], [-0.155432758, 51.4934983005], [-0.1556536853, 51.4936065998], [-0.1559241899, 51.4936538801], [-0.1562030893, 51.4936329433], [-0.1573164311, 51.4931897744], [-0.1579570413, 51.4931170608], [-0.1581784603, 51.4930499167], [-0.1583835504, 51.4929074402], [-0.1584777328, 51.4926860385]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+        </is>
+      </c>
+      <c r="Z35" t="inlineStr">
+        <is>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3216] SLOANE SQUARE (SW1W,SW1X,SW3)', 'closure': 'Closed', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.156313,51.493054],[-0.155979,51.493206]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157034,51.492764],[-0.15677,51.492877]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157758,51.492685],[-0.157034,51.492764]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.15677,51.492877],[-0.156313,51.493054]]', 'sourceSystemId': 0}], 'sourceSystemId': 206069, 'sourceSystemKey': 'TIMS'}]</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4634,17 +4642,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>TIMS-206069</t>
+          <t>TIMS-204963</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206069</t>
+          <t>/Road/All/Disruption/TIMS-204963</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>[-0.156729,51.49289]</t>
+          <t>[-0.051059,51.497108]</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -4667,17 +4675,17 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>[A3216] Sloane Square (Eastbound) at the junction of Sedding Street - Road is closed due to emergency Thames Water and Cadent Gas works</t>
+          <t xml:space="preserve">Surrey Quays Road (Both directions) between [A200] Lower Road and Deal Porters Way - Road closure due to UKPN works. </t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Use an alternative route. There are no reported delays on diversion.</t>
+          <t>Use an alternative route. Delays are possible on diversion.</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-01-22T17:51:06Z</t>
+          <t>2025-01-22T09:32:28Z</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -4687,17 +4695,17 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>2025-01-20T10:00:00Z</t>
+          <t>2025-01-06T08:00:00Z</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>2025-01-25T18:00:00Z</t>
+          <t>2025-01-27T23:59:00Z</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>2025-01-22T18:50:15Z</t>
+          <t>2025-01-22T09:32:28Z</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -4707,7 +4715,7 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>[A3216] SLOANE SQUARE (SW1W,SW1X,SW3) (Kensington &amp; Chelsea,Westminster)</t>
+          <t>SURREY QUAYS ROAD (SE16) (Southwark)</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -4717,7 +4725,7 @@
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.156729, 51.49289], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.051059, 51.497108], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T36" t="b">
@@ -4743,12 +4751,12 @@
       </c>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>{'type': 'Polygon', 'coordinates': [[[-0.1584777328, 51.4926860385], [-0.1584390066, 51.4925397983], [-0.1583261769, 51.4924093762], [-0.1581841856, 51.4923230989], [-0.1579722888, 51.4922562091], [-0.1576578673, 51.4922401505], [-0.1567956082, 51.4923397904], [-0.1558023405, 51.4927240695], [-0.1554594231, 51.4928949283], [-0.1552773642, 51.4931060012], [-0.1552950424, 51.4933454702], [-0.155432758, 51.4934983005], [-0.1556536853, 51.4936065998], [-0.1559241899, 51.4936538801], [-0.1562030893, 51.4936329433], [-0.1573164311, 51.4931897744], [-0.1579570413, 51.4931170608], [-0.1581784603, 51.4930499167], [-0.1583835504, 51.4929074402], [-0.1584777328, 51.4926860385]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Polygon', 'coordinates': [[[-0.0532202117, 51.4963035624], [-0.0531101128, 51.4960739009], [-0.0528690697, 51.4959268849], [-0.0525472474, 51.4958644434], [-0.0521712196, 51.4959132037], [-0.0516174361, 51.4961298027], [-0.0503558083, 51.4967719877], [-0.0498691758, 51.496890246], [-0.0495415109, 51.4970175148], [-0.0493385719, 51.4971906357], [-0.0492507999, 51.4973265335], [-0.0492421467, 51.4974936739], [-0.0493156798, 51.4976328251], [-0.0495914138, 51.4978127893], [-0.0499783293, 51.4978734978], [-0.0502397027, 51.4978367444], [-0.050501731, 51.4977155507], [-0.0509786307, 51.4975883274], [-0.0516983202, 51.4972665459], [-0.0524610818, 51.4968615851], [-0.052981877, 51.4966470183], [-0.0531610554, 51.4964915146], [-0.0532202117, 51.4963035624]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3216] SLOANE SQUARE (SW1W,SW1X,SW3)', 'closure': 'Closed', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.156313,51.493054],[-0.155979,51.493206]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157034,51.492764],[-0.15677,51.492877]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157758,51.492685],[-0.157034,51.492764]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.15677,51.492877],[-0.156313,51.493054]]', 'sourceSystemId': 0}], 'sourceSystemId': 206069, 'sourceSystemKey': 'TIMS'}]</t>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'SURREY QUAYS ROAD (SE16)', 'closure': 'Closed', 'directions': 'Both directions', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.0525,51.496313],[-0.052391,51.49636]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.049954,51.497424],[-0.050301,51.497284]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052391,51.49636],[-0.052173,51.496447]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052039,51.496494],[-0.050301,51.497284]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052173,51.496447],[-0.052039,51.496494]]', 'sourceSystemId': 0}], 'sourceSystemId': 204963, 'sourceSystemKey': 'TIMS'}]</t>
         </is>
       </c>
     </row>
@@ -4886,17 +4894,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>TIMS-204963</t>
+          <t>TIMS-206054</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204963</t>
+          <t>/Road/All/Disruption/TIMS-206054</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>[-0.051059,51.497108]</t>
+          <t>[-0.12737,51.509315]</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -4919,17 +4927,17 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Surrey Quays Road (Both directions) between [A200] Lower Road and Deal Porters Way - Road closure due to UKPN works. </t>
+          <t>[A400] St Martins Place (All directions) at the junction of [A400] Charing Cross Road - Temporary signals in operation to facilitate Cadent Gas works.</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Use an alternative route. Delays are possible on diversion.</t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-01-22T09:32:28Z</t>
+          <t>2025-01-22T17:51:14Z</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -4939,17 +4947,17 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>2025-01-06T08:00:00Z</t>
+          <t>2025-01-19T17:45:00Z</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>2025-01-27T23:59:00Z</t>
+          <t>2025-01-24T17:00:00Z</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>2025-01-22T09:32:28Z</t>
+          <t>2025-01-22T17:51:14Z</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -4959,7 +4967,7 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>SURREY QUAYS ROAD (SE16) (Southwark)</t>
+          <t>[A400] ST MARTINS PLACE (WC2N) (Westminster)</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -4969,7 +4977,7 @@
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.051059, 51.497108], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.12737, 51.509315], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T38" t="b">
@@ -4993,16 +5001,8 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y38" t="inlineStr">
-        <is>
-          <t>{'type': 'Polygon', 'coordinates': [[[-0.0532202117, 51.4963035624], [-0.0531101128, 51.4960739009], [-0.0528690697, 51.4959268849], [-0.0525472474, 51.4958644434], [-0.0521712196, 51.4959132037], [-0.0516174361, 51.4961298027], [-0.0503558083, 51.4967719877], [-0.0498691758, 51.496890246], [-0.0495415109, 51.4970175148], [-0.0493385719, 51.4971906357], [-0.0492507999, 51.4973265335], [-0.0492421467, 51.4974936739], [-0.0493156798, 51.4976328251], [-0.0495914138, 51.4978127893], [-0.0499783293, 51.4978734978], [-0.0502397027, 51.4978367444], [-0.050501731, 51.4977155507], [-0.0509786307, 51.4975883274], [-0.0516983202, 51.4972665459], [-0.0524610818, 51.4968615851], [-0.052981877, 51.4966470183], [-0.0531610554, 51.4964915146], [-0.0532202117, 51.4963035624]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="Z38" t="inlineStr">
-        <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'SURREY QUAYS ROAD (SE16)', 'closure': 'Closed', 'directions': 'Both directions', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.0525,51.496313],[-0.052391,51.49636]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.049954,51.497424],[-0.050301,51.497284]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052391,51.49636],[-0.052173,51.496447]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052039,51.496494],[-0.050301,51.497284]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052173,51.496447],[-0.052039,51.496494]]', 'sourceSystemId': 0}], 'sourceSystemId': 204963, 'sourceSystemKey': 'TIMS'}]</t>
-        </is>
-      </c>
+      <c r="Y38" t="inlineStr"/>
+      <c r="Z38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5012,17 +5012,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>TIMS-205898</t>
+          <t>TIMS-203041</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205898</t>
+          <t>/Road/All/Disruption/TIMS-203041</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>[0.000174,51.458561]</t>
+          <t>[-0.010106,51.461524]</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -5040,42 +5040,42 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>Borough works</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>[A20] Lee High Road (Both directions) at the junction of Glenton Road - Two-way temporary traffic signals in place to facilitate SGN works.</t>
+          <t>Lewisham High Street (Northbound) at the junction of Lewis Grove - Road closure northbound between Lewisham High Street and Lee Bridge to facilitate works.</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t>Use an alternative route. Delays are possible on diversion.</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-01-22T09:26:00Z</t>
+          <t>2025-01-22T09:31:03Z</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>['a20']</t>
+          <t>['a20', 'a21']</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>2025-01-15T12:05:00Z</t>
+          <t>2024-08-03T07:00:00Z</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>2025-01-23T23:59:00Z</t>
+          <t>2025-03-31T17:00:00Z</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>2025-01-22T09:26:00Z</t>
+          <t>2025-01-22T09:31:14Z</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -5085,7 +5085,7 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>[A20] LEE HIGH ROAD (SE12,SE13,SE3) (Lewisham)</t>
+          <t>LEWISHAM HIGH STREET (SE13) (Lewisham)</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -5095,7 +5095,7 @@
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [0.000174, 51.458561], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.010106, 51.461524], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T39" t="b">
@@ -5119,8 +5119,16 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y39" t="inlineStr"/>
-      <c r="Z39" t="inlineStr"/>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>{'type': 'Polygon', 'coordinates': [[[-0.012734878, 51.4593126239], [-0.0126900506, 51.4591409421], [-0.0125806121, 51.4590193676], [-0.0124167755, 51.4589246095], [-0.0122143225, 51.4588657953], [-0.011992754, 51.4588485902], [-0.0117734125, 51.4588746513], [-0.0115774255, 51.4589414685], [-0.0113907291, 51.4590667721], [-0.0111057165, 51.4594449735], [-0.010635101, 51.459946833], [-0.0099789336, 51.4607894854], [-0.009678438, 51.4610565384], [-0.009604918, 51.4611951152], [-0.0093358373, 51.4612878686], [-0.0091500677, 51.4614469781], [-0.0086289053, 51.462360547], [-0.008690566, 51.4625971575], [-0.0089381945, 51.4627803029], [-0.0091964122, 51.4628490915], [-0.0094771174, 51.4628509183], [-0.0097375735, 51.4627855052], [-0.009938127, 51.4626628111], [-0.0105206374, 51.4616962362], [-0.0108456493, 51.4615692905], [-0.0112195757, 51.4612465742], [-0.0120015704, 51.4602565133], [-0.0124604446, 51.4597553773], [-0.0126555264, 51.4596022293], [-0.0127163805, 51.4594883868], [-0.012734878, 51.4593126239]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+        </is>
+      </c>
+      <c r="Z39" t="inlineStr">
+        <is>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'LEWIS GROVE (SE13)', 'closure': 'Closed', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.009344,51.462409],[-0.00981,51.461626]]', 'sourceSystemId': 0}], 'sourceSystemId': 203041, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A21] LEWISHAM HIGH STREET (SE13)', 'closure': 'Closed', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.012008,51.459406],[-0.012016,51.459298]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010315,51.461266],[-0.010405,51.461195]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010405,51.461195],[-0.010736,51.46085]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.011773,51.459625],[-0.012016,51.459298]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.011773,51.459625],[-0.010951,51.460548]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010951,51.460548],[-0.010736,51.46085]]', 'sourceSystemId': 0}], 'sourceSystemId': 203041, 'sourceSystemKey': 'TIMS'}]</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5130,17 +5138,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>TIMS-203041</t>
+          <t>TIMS-205742</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-203041</t>
+          <t>/Road/All/Disruption/TIMS-205742</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[-0.010106,51.461524]</t>
+          <t>[-0.063863,51.473961]</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -5158,42 +5166,42 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Borough works</t>
+          <t>TfL works</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Lewisham High Street (Northbound) at the junction of Lewis Grove - Road closure northbound between Lewisham High Street and Lee Bridge to facilitate works.</t>
+          <t>[A202] Peckham High Street (Southbound) between Consort Road and [A2215] Clayton Road - Southbound lane closures in operation to facilitate maintenance works.</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Use an alternative route. Delays are possible on diversion.</t>
+          <t>Some delays maybe experienced while this work takes place.</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-01-22T09:31:03Z</t>
+          <t>2025-01-22T20:07:37Z</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>['a20', 'a21']</t>
+          <t>['a20']</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>2024-08-03T07:00:00Z</t>
+          <t>2025-01-22T20:00:00Z</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>2025-03-31T17:00:00Z</t>
+          <t>2025-01-23T06:00:00Z</t>
         </is>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>2025-01-22T09:31:14Z</t>
+          <t>2025-01-22T20:07:39Z</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -5203,7 +5211,7 @@
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>LEWISHAM HIGH STREET (SE13) (Lewisham)</t>
+          <t>[A202] PECKHAM HIGH STREET (SE15) (Southwark)</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -5213,7 +5221,7 @@
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.010106, 51.461524], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.063863, 51.473961], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T40" t="b">
@@ -5237,16 +5245,8 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y40" t="inlineStr">
-        <is>
-          <t>{'type': 'Polygon', 'coordinates': [[[-0.012734878, 51.4593126239], [-0.0126900506, 51.4591409421], [-0.0125806121, 51.4590193676], [-0.0124167755, 51.4589246095], [-0.0122143225, 51.4588657953], [-0.011992754, 51.4588485902], [-0.0117734125, 51.4588746513], [-0.0115774255, 51.4589414685], [-0.0113907291, 51.4590667721], [-0.0111057165, 51.4594449735], [-0.010635101, 51.459946833], [-0.0099789336, 51.4607894854], [-0.009678438, 51.4610565384], [-0.009604918, 51.4611951152], [-0.0093358373, 51.4612878686], [-0.0091500677, 51.4614469781], [-0.0086289053, 51.462360547], [-0.008690566, 51.4625971575], [-0.0089381945, 51.4627803029], [-0.0091964122, 51.4628490915], [-0.0094771174, 51.4628509183], [-0.0097375735, 51.4627855052], [-0.009938127, 51.4626628111], [-0.0105206374, 51.4616962362], [-0.0108456493, 51.4615692905], [-0.0112195757, 51.4612465742], [-0.0120015704, 51.4602565133], [-0.0124604446, 51.4597553773], [-0.0126555264, 51.4596022293], [-0.0127163805, 51.4594883868], [-0.012734878, 51.4593126239]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="Z40" t="inlineStr">
-        <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'LEWIS GROVE (SE13)', 'closure': 'Closed', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.009344,51.462409],[-0.00981,51.461626]]', 'sourceSystemId': 0}], 'sourceSystemId': 203041, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A21] LEWISHAM HIGH STREET (SE13)', 'closure': 'Closed', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.012008,51.459406],[-0.012016,51.459298]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010315,51.461266],[-0.010405,51.461195]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010405,51.461195],[-0.010736,51.46085]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.011773,51.459625],[-0.012016,51.459298]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.011773,51.459625],[-0.010951,51.460548]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010951,51.460548],[-0.010736,51.46085]]', 'sourceSystemId': 0}], 'sourceSystemId': 203041, 'sourceSystemKey': 'TIMS'}]</t>
-        </is>
-      </c>
+      <c r="Y40" t="inlineStr"/>
+      <c r="Z40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5256,17 +5256,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>TIMS-205742</t>
+          <t>TIMS-205898</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205742</t>
+          <t>/Road/All/Disruption/TIMS-205898</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>[-0.063863,51.473961]</t>
+          <t>[0.000174,51.458561]</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -5284,22 +5284,22 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>TfL works</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>[A202] Peckham High Street (Southbound) between Consort Road and [A2215] Clayton Road - Southbound lane closures in operation to facilitate maintenance works.</t>
+          <t>[A20] Lee High Road (Both directions) at the junction of Glenton Road - Two-way temporary traffic signals in place to facilitate SGN works.</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Some delays maybe experienced while this work takes place.</t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-01-22T20:07:37Z</t>
+          <t>2025-01-22T09:26:00Z</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -5309,17 +5309,17 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>2025-01-22T20:00:00Z</t>
+          <t>2025-01-15T12:05:00Z</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>2025-01-23T06:00:00Z</t>
+          <t>2025-01-23T23:59:00Z</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>2025-01-22T20:07:39Z</t>
+          <t>2025-01-22T09:26:00Z</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>[A202] PECKHAM HIGH STREET (SE15) (Southwark)</t>
+          <t>[A20] LEE HIGH ROAD (SE12,SE13,SE3) (Lewisham)</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -5339,7 +5339,7 @@
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.063863, 51.473961], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [0.000174, 51.458561], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T41" t="b">
@@ -5374,17 +5374,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>TIMS-205940</t>
+          <t>TIMS-206068</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205940</t>
+          <t>/Road/All/Disruption/TIMS-206068</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>[-0.021394,51.444843]</t>
+          <t>[-0.193207,51.457005]</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -5397,27 +5397,27 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Planned events</t>
+          <t>Works</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Demonstration/March</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Pro-Palestine Demonstration - [A205] Catford Road (All approaches) at the junction of [A21] Rushey Green - Pro-Palestine Demonstration. Expect an increase in pedestrians and traffic before and after the event.</t>
+          <t>[A3] Wandsworth High Street (Westbound) at the junction of [A217] Ram Street - Lanes two and three (of three) is blocked due to emergency Thames Water works.</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Expect an increase in pedestrians and traffic before and after the event.</t>
+          <t>Traffic is flowing well past the works.</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-01-22T19:02:28Z</t>
+          <t>2025-01-22T19:11:19Z</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -5427,17 +5427,17 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>2025-01-22T18:30:00Z</t>
+          <t>2025-01-20T10:05:00Z</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>2025-01-22T21:00:00Z</t>
+          <t>2025-02-04T18:00:00Z</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>2025-01-22T19:02:30Z</t>
+          <t>2025-01-22T19:11:19Z</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -5447,7 +5447,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>[A205] CATFORD ROAD (SE14,SE6) (Lewisham)</t>
+          <t>[A3] WANDSWORTH HIGH STREET (SW18) (Wandsworth)</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -5457,7 +5457,7 @@
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.021394, 51.444843], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.193207, 51.457005], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T42" t="b">
@@ -5610,17 +5610,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>TIMS-206068</t>
+          <t>TIMS-205629</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206068</t>
+          <t>/Road/All/Disruption/TIMS-205629</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>[-0.193207,51.457005]</t>
+          <t>[-0.253857,51.437053]</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -5643,37 +5643,37 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>[A3] Wandsworth High Street (Westbound) at the junction of [A217] Ram Street - Lanes two and three (of three) is blocked due to emergency Thames Water works.</t>
+          <t>[A3] Roehampton Vale (Westbound) at the junction of [A3] Kingston Vale - Thames Water works. The slip road from westbound A3 Roehampton Vale into A308 Kingston Vale is closed.</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Traffic is flowing well past the works.</t>
+          <t>Use an alternative route. Delays are possible.</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-01-22T19:11:19Z</t>
+          <t>2025-01-22T09:41:10Z</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>['a205']</t>
+          <t>['a3']</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>2025-01-20T10:05:00Z</t>
+          <t>2025-01-08T16:45:00Z</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>2025-02-04T18:00:00Z</t>
+          <t>2025-01-29T17:00:00Z</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>2025-01-22T19:11:19Z</t>
+          <t>2025-01-22T09:41:22Z</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -5683,7 +5683,7 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>[A3] WANDSWORTH HIGH STREET (SW18) (Wandsworth)</t>
+          <t>[A3] ROEHAMPTON VALE (SW15) (Kingston upon Thames,Wandsworth)</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -5693,7 +5693,7 @@
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.193207, 51.457005], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.253857, 51.437053], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T44" t="b">
@@ -5728,17 +5728,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TIMS-205629</t>
+          <t>TIMS-206145</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205629</t>
+          <t>/Road/All/Disruption/TIMS-206145</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>[-0.253857,51.437053]</t>
+          <t>[-0.198331,51.491627]</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -5761,37 +5761,37 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>[A3] Roehampton Vale (Westbound) at the junction of [A3] Kingston Vale - Thames Water works. The slip road from westbound A3 Roehampton Vale into A308 Kingston Vale is closed.</t>
+          <t>[A3220] Warwick Road (Northbound) at the junction of Nevern Square - Lane closure in place to facilitate UKPN works.</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Use an alternative route. Delays are possible.</t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-01-22T09:41:10Z</t>
+          <t>2025-01-22T17:50:55Z</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>['a3']</t>
+          <t>['a4', 'western cross route']</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>2025-01-08T16:45:00Z</t>
+          <t>2025-01-22T08:00:00Z</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>2025-01-29T17:00:00Z</t>
+          <t>2025-02-05T18:00:00Z</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>2025-01-22T09:41:22Z</t>
+          <t>2025-01-22T17:50:55Z</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -5801,7 +5801,7 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>[A3] ROEHAMPTON VALE (SW15) (Kingston upon Thames,Wandsworth)</t>
+          <t>[A3220] WARWICK ROAD (SW10,SW5,W14,W8) (Kensington &amp; Chelsea)</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -5811,7 +5811,7 @@
       </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.253857, 51.437053], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.198331, 51.491627], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T45" t="b">
@@ -5846,17 +5846,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TIMS-206145</t>
+          <t>TIMS-205539</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206145</t>
+          <t>/Road/All/Disruption/TIMS-205539</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[-0.198331,51.491627]</t>
+          <t>[-0.167464,51.518121]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -5879,7 +5879,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>[A3220] Warwick Road (Northbound) at the junction of Nevern Square - Lane closure in place to facilitate UKPN works.</t>
+          <t>[A5] Edgware Road (Southbound) at the junction of [A501] Old Marylebone Road - Lane one (of two ) closure due to utility works</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -5889,27 +5889,27 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-01-22T17:50:55Z</t>
+          <t>2025-01-22T20:05:46Z</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>['a4', 'western cross route']</t>
+          <t>['a40', 'a41', 'inner ring']</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>2025-01-22T08:00:00Z</t>
+          <t>2025-01-22T20:01:00Z</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>2025-02-05T18:00:00Z</t>
+          <t>2025-01-23T06:00:00Z</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>2025-01-22T17:50:55Z</t>
+          <t>2025-01-22T20:05:48Z</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -5919,7 +5919,7 @@
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>[A3220] WARWICK ROAD (SW10,SW5,W14,W8) (Kensington &amp; Chelsea)</t>
+          <t>[A5] EDGWARE ROAD (NW1,NW8,W1H,W2) (Westminster)</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
@@ -5929,7 +5929,7 @@
       </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.198331, 51.491627], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.167464, 51.518121], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T46" t="b">
@@ -5964,17 +5964,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>TIMS-205539</t>
+          <t>TIMS-205970</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205539</t>
+          <t>/Road/All/Disruption/TIMS-205970</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>[-0.167464,51.518121]</t>
+          <t>[-0.280535,51.47514]</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -5997,37 +5997,37 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>[A5] Edgware Road (Southbound) at the junction of [A501] Old Marylebone Road - Lane one (of two ) closure due to utility works</t>
+          <t>[A205] Mortlake Road (Both directions) at the junction of High Park Road - Road is closed in both directions to allow for essential road maintenance to be carried out by Thames Water</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Traffic is flowing well.</t>
+          <t>Use an alternative route. Delays are possible on diversion.</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-01-22T20:05:46Z</t>
+          <t>2025-01-22T09:39:37Z</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>['a40', 'a41', 'inner ring']</t>
+          <t>['a406']</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>2025-01-22T20:01:00Z</t>
+          <t>2025-01-16T17:55:00Z</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>2025-01-23T06:00:00Z</t>
+          <t>2025-01-22T23:59:00Z</t>
         </is>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>2025-01-22T20:05:48Z</t>
+          <t>2025-01-22T09:39:48Z</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -6037,7 +6037,7 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>[A5] EDGWARE ROAD (NW1,NW8,W1H,W2) (Westminster)</t>
+          <t>[A205] MORTLAKE ROAD (SW14,TW9) (Richmond upon Thames)</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
@@ -6047,7 +6047,7 @@
       </c>
       <c r="S47" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.167464, 51.518121], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.280535, 51.47514], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T47" t="b">
@@ -6072,7 +6072,11 @@
         </is>
       </c>
       <c r="Y47" t="inlineStr"/>
-      <c r="Z47" t="inlineStr"/>
+      <c r="Z47" t="inlineStr">
+        <is>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A205] MORTLAKE ROAD (TW9)', 'closure': 'Closed', 'directions': 'Both directions', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206507009', 'lineString': '[[-0.279734,51.474789],[-0.279608,51.474739]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206507010', 'lineString': '[[-0.279608,51.474739],[-0.279444,51.474692]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206509263', 'lineString': '[[-0.279792,51.474818],[-0.279734,51.474789]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}], 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}]</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6082,17 +6086,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>TIMS-205970</t>
+          <t>TIMS-204896</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205970</t>
+          <t>/Road/All/Disruption/TIMS-204896</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>[-0.280535,51.47514]</t>
+          <t>[-0.174162,51.53443]</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -6115,37 +6119,37 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>[A205] Mortlake Road (Both directions) at the junction of High Park Road - Road is closed in both directions to allow for essential road maintenance to be carried out by Thames Water</t>
+          <t>Utility Works - Thames Water - [A41] Finchley Road (Both directions) at the junction of [A41] Wellington Road - Side road closures will be implemented with local diversions from the 6th of January to 3rd February to allow for water works by Thames Water.</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Use an alternative route. Delays are possible on diversion.</t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-01-22T09:39:37Z</t>
+          <t>2025-01-22T13:37:57Z</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>['a406']</t>
+          <t>['a41']</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>2025-01-16T17:55:00Z</t>
+          <t>2025-01-12T08:00:00Z</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>2025-01-22T23:59:00Z</t>
+          <t>2025-01-12T18:00:00Z</t>
         </is>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>2025-01-22T09:39:48Z</t>
+          <t>2025-01-22T13:38:24Z</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -6155,7 +6159,7 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>[A205] MORTLAKE ROAD (SW14,TW9) (Richmond upon Thames)</t>
+          <t>[A41] FINCHLEY ROAD (NW8) (Camden,Westminster)</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
@@ -6165,7 +6169,7 @@
       </c>
       <c r="S48" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.280535, 51.47514], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.174162, 51.53443], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T48" t="b">
@@ -6190,11 +6194,7 @@
         </is>
       </c>
       <c r="Y48" t="inlineStr"/>
-      <c r="Z48" t="inlineStr">
-        <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A205] MORTLAKE ROAD (TW9)', 'closure': 'Closed', 'directions': 'Both directions', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206507009', 'lineString': '[[-0.279734,51.474789],[-0.279608,51.474739]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206507010', 'lineString': '[[-0.279608,51.474739],[-0.279444,51.474692]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206509263', 'lineString': '[[-0.279792,51.474818],[-0.279734,51.474789]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}], 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}]</t>
-        </is>
-      </c>
+      <c r="Z48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -6204,17 +6204,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>TIMS-204896</t>
+          <t>TIMS-205973</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204896</t>
+          <t>/Road/All/Disruption/TIMS-205973</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[-0.174162,51.53443]</t>
+          <t>[-0.084093,51.513343]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -6232,42 +6232,42 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>TfL works</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Utility Works - Thames Water - [A41] Finchley Road (Both directions) at the junction of [A41] Wellington Road - Side road closures will be implemented with local diversions from the 6th of January to 3rd February to allow for water works by Thames Water.</t>
+          <t>[A10] Gracechurch Street (Both directions) at the junction of Leadenhall Street - Lane restrictions to facilitate collaborative works.</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Traffic is flowing well.</t>
+          <t xml:space="preserve">There are no reported delays. </t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-01-22T13:37:57Z</t>
+          <t>2025-01-22T17:51:27Z</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>['a41']</t>
+          <t>['bishopsgate cross route']</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>2025-01-12T08:00:00Z</t>
+          <t>2025-01-20T08:00:00Z</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>2025-01-12T18:00:00Z</t>
+          <t>2025-01-31T17:00:00Z</t>
         </is>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>2025-01-22T13:38:24Z</t>
+          <t>2025-01-22T17:51:27Z</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -6277,7 +6277,7 @@
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>[A41] FINCHLEY ROAD (NW8) (Camden,Westminster)</t>
+          <t>[A10] GRACECHURCH STREET (EC3V,EC4N,EC4R) (City of London)</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -6287,7 +6287,7 @@
       </c>
       <c r="S49" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.174162, 51.53443], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.084093, 51.513343], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T49" t="b">
@@ -6322,17 +6322,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>TIMS-205973</t>
+          <t>TIMS-204461</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205973</t>
+          <t>/Road/All/Disruption/TIMS-204461</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>[-0.084093,51.513343]</t>
+          <t>[-0.122625,51.494512]</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -6355,37 +6355,37 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>[A10] Gracechurch Street (Both directions) at the junction of Leadenhall Street - Lane restrictions to facilitate collaborative works.</t>
+          <t xml:space="preserve">[A3203] Lambeth Bridge (Both directions) between [A3212] Millbank and [A3036] A 3036 - Various restrictions during junction improvement works at either side of Lambeth Bridge. Currently restrictions are in place on all approaches and inner ring of Lambeth Roundabout. From 30 January 21:30 until 07 February 05:00, there will be nightly road closures of Lambeth Bridge, Lambeth Palace Road, Lambeth Road &amp; Albert Embankment, with diversions in place via Westminster and Vauxhall Bridges. </t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t xml:space="preserve">There are no reported delays. </t>
+          <t xml:space="preserve">Delays are possible. </t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-01-22T17:51:27Z</t>
+          <t>2025-01-22T08:05:25Z</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>['bishopsgate cross route']</t>
+          <t>['southern river route']</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>2025-01-20T08:00:00Z</t>
+          <t>2024-08-31T23:01:00Z</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>2025-01-31T17:00:00Z</t>
+          <t>2025-05-08T16:00:00Z</t>
         </is>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>2025-01-22T17:51:27Z</t>
+          <t>2025-01-22T08:05:34Z</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -6395,7 +6395,7 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>[A10] GRACECHURCH STREET (EC3V,EC4N,EC4R) (City of London)</t>
+          <t>[A3203] LAMBETH BRIDGE (SE1,SW1P) (Lambeth,Westminster)</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -6405,7 +6405,7 @@
       </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.084093, 51.513343], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.122625, 51.494512], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T50" t="b">
@@ -6558,17 +6558,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>TIMS-204461</t>
+          <t>TIMS-205916</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204461</t>
+          <t>/Road/All/Disruption/TIMS-205916</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>[-0.122625,51.494512]</t>
+          <t>[-0.343052,51.542371]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -6586,42 +6586,42 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>TfL works</t>
+          <t>Borough works</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t xml:space="preserve">[A3203] Lambeth Bridge (Both directions) between [A3212] Millbank and [A3036] A 3036 - Various restrictions during junction improvement works at either side of Lambeth Bridge. Currently restrictions are in place on all approaches and inner ring of Lambeth Roundabout. From 30 January 21:30 until 07 February 05:00, there will be nightly road closures of Lambeth Bridge, Lambeth Palace Road, Lambeth Road &amp; Albert Embankment, with diversions in place via Westminster and Vauxhall Bridges. </t>
+          <t>[A4127] Greenford Road (Both directions) at the junction of Rockware Avenue - Temporary traffic signals in place to facilitate roadworks</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delays are possible. </t>
+          <t>Traffic is slow moving in the area</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2025-01-22T08:05:25Z</t>
+          <t>2025-01-22T13:39:43Z</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>['southern river route']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>2024-08-31T23:01:00Z</t>
+          <t>2025-01-20T08:00:00Z</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>2025-05-08T16:00:00Z</t>
+          <t>2025-01-27T06:00:00Z</t>
         </is>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>2025-01-22T08:05:34Z</t>
+          <t>2025-01-22T16:55:22Z</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -6631,7 +6631,7 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>[A3203] LAMBETH BRIDGE (SE1,SW1P) (Lambeth,Westminster)</t>
+          <t>[A4127] GREENFORD ROAD (UB5,UB6) (Ealing)</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -6641,7 +6641,7 @@
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.122625, 51.494512], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.343052, 51.542371], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T52" t="b">
@@ -6676,17 +6676,17 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>TIMS-205512</t>
+          <t>TIMS-205243</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205512</t>
+          <t>/Road/All/Disruption/TIMS-205243</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>[-0.106039,51.556345]</t>
+          <t>[-0.100283,51.493373]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -6699,27 +6699,27 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Planned events</t>
+          <t>Works</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Sporting</t>
+          <t>Construction activity</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>Drayton Park (All approaches) at the junction of Aubert Park - Arsenal v Dynamo Zagreb Football Match.</t>
+          <t>[A215] Walworth Road (Southbound) at the junction of [A3] Newington Butts - Lane restriction contained to southbound Walworth Road to facilitate scaffolding works.</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delays possible. </t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>2025-01-22T19:21:18Z</t>
+          <t>2025-01-22T08:12:06Z</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -6729,17 +6729,17 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>2025-01-22T19:00:00Z</t>
+          <t>2025-01-13T08:00:00Z</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>2025-01-22T22:30:00Z</t>
+          <t>2025-10-03T22:59:00Z</t>
         </is>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>2025-01-22T19:21:21Z</t>
+          <t>2025-01-22T08:17:28Z</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -6749,7 +6749,7 @@
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>DRAYTON PARK (N5,N7) (Islington)</t>
+          <t>[A215] WALWORTH ROAD (SE1,SE17) (Southwark)</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -6759,7 +6759,7 @@
       </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.106039, 51.556345], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.100283, 51.493373], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T53" t="b">
@@ -6794,17 +6794,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>TIMS-205916</t>
+          <t>TIMS-206136</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205916</t>
+          <t>/Road/All/Disruption/TIMS-206136</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>[-0.343052,51.542371]</t>
+          <t>[-0.170834,51.51835]</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -6827,17 +6827,17 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>[A4127] Greenford Road (Both directions) at the junction of Rockware Avenue - Temporary traffic signals in place to facilitate roadworks</t>
+          <t>[A4205] Praed Street (Both directions) at the junction of Sale Place - Road works are being carried out at this location under temporary signals.</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Traffic is slow moving in the area</t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>2025-01-22T13:39:43Z</t>
+          <t>2025-01-22T07:06:04Z</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -6847,17 +6847,17 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>2025-01-20T08:00:00Z</t>
+          <t>2025-01-22T00:04:00Z</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>2025-01-27T06:00:00Z</t>
+          <t>2025-01-27T23:59:00Z</t>
         </is>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>2025-01-22T16:55:22Z</t>
+          <t>2025-01-22T07:06:38Z</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -6867,7 +6867,7 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>[A4127] GREENFORD ROAD (UB5,UB6) (Ealing)</t>
+          <t>[A4205] PRAED STREET (W2) (Westminster)</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -6877,7 +6877,7 @@
       </c>
       <c r="S54" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.343052, 51.542371], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.170834, 51.51835], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T54" t="b">
@@ -6912,17 +6912,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>TIMS-206136</t>
+          <t>TIMS-205512</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206136</t>
+          <t>/Road/All/Disruption/TIMS-205512</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>[-0.170834,51.51835]</t>
+          <t>[-0.106039,51.556345]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -6935,27 +6935,27 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Works</t>
+          <t>Planned events</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Borough works</t>
+          <t>Sporting</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>[A4205] Praed Street (Both directions) at the junction of Sale Place - Road works are being carried out at this location under temporary signals.</t>
+          <t>Drayton Park (All approaches) at the junction of Aubert Park - Arsenal v Dynamo Zagreb Football Match.</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t xml:space="preserve">Delays possible. </t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>2025-01-22T07:06:04Z</t>
+          <t>2025-01-22T19:21:18Z</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -6965,17 +6965,17 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>2025-01-22T00:04:00Z</t>
+          <t>2025-01-22T19:00:00Z</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>2025-01-27T23:59:00Z</t>
+          <t>2025-01-22T22:30:00Z</t>
         </is>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>2025-01-22T07:06:38Z</t>
+          <t>2025-01-22T19:21:21Z</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -6985,7 +6985,7 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>[A4205] PRAED STREET (W2) (Westminster)</t>
+          <t>DRAYTON PARK (N5,N7) (Islington)</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -6995,7 +6995,7 @@
       </c>
       <c r="S55" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.170834, 51.51835], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.106039, 51.556345], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T55" t="b">
@@ -7021,124 +7021,6 @@
       </c>
       <c r="Y55" t="inlineStr"/>
       <c r="Z55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Tfl.Api.Presentation.Entities.RoadDisruption, Tfl.Api.Presentation.Entities</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>TIMS-205243</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>/Road/All/Disruption/TIMS-205243</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>[-0.100283,51.493373]</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>Minimal</t>
-        </is>
-      </c>
-      <c r="F56" t="n">
-        <v>55</v>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>Works</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>Construction activity</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>[A215] Walworth Road (Southbound) at the junction of [A3] Newington Butts - Lane restriction contained to southbound Walworth Road to facilitate scaffolding works.</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>Delays are possible.</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>2025-01-22T08:12:06Z</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>2025-01-13T08:00:00Z</t>
-        </is>
-      </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>2025-10-03T22:59:00Z</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>2025-01-22T08:17:28Z</t>
-        </is>
-      </c>
-      <c r="P56" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>[A215] WALWORTH ROAD (SE1,SE17) (Southwark)</t>
-        </is>
-      </c>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>{'type': 'Point', 'coordinates': [-0.100283, 51.493373], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="T56" t="b">
-        <v>0</v>
-      </c>
-      <c r="U56" t="b">
-        <v>0</v>
-      </c>
-      <c r="V56" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="W56" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="X56" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="Y56" t="inlineStr"/>
-      <c r="Z56" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed KeyError by updating severity and comments keys in analysis, and other changes
</commit_message>
<xml_diff>
--- a/disruptions.xlsx
+++ b/disruptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z55"/>
+  <dimension ref="A1:Z53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -734,7 +734,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-01-22T19:47:42Z</t>
+          <t>2025-01-22T20:57:24Z</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>2025-01-22T19:47:42Z</t>
+          <t>2025-01-22T20:57:24Z</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -880,7 +880,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>2025-01-22T19:13:31Z</t>
+          <t>2025-01-22T21:33:09Z</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -2132,17 +2132,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TIMS-200121</t>
+          <t>TIMS-205721</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-200121</t>
+          <t>/Road/All/Disruption/TIMS-205721</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[-0.008204,51.507309]</t>
+          <t>[-0.287669,51.553499]</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -2160,22 +2160,22 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>TfL works</t>
+          <t>Borough works</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Silvertown Tunnel Scheme - Preston's Roundabout - [A1206] Prestons Road Roundabout (All directions) between [A1206] Prestons Road and [A1261] Aspen Way - Lane restrictions are in place to facilitate Silvertown Tunnel related works.</t>
+          <t>[A404] High Road (Both directions) at the junction of [B4565] Wembley Hill Road - Temporary traffic signals in place to facilitate roadworks.</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t>There are no reported delays</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-01-22T13:38:22Z</t>
+          <t>2025-01-22T20:35:13Z</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -2185,17 +2185,17 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>2024-09-16T06:00:00Z</t>
+          <t>2025-01-13T05:00:00Z</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2025-03-01T19:00:00Z</t>
+          <t>2025-05-19T17:00:00Z</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>2025-01-22T13:38:22Z</t>
+          <t>2025-01-22T20:35:13Z</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>[A1206] PRESTONS ROAD ROUNDABOUT (E14) (Tower Hamlets)</t>
+          <t>[A404] HIGH ROAD (HA9) (Brent)</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -2215,7 +2215,7 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.008204, 51.507309], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.287669, 51.553499], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T15" t="b">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>TIMS-199419</t>
+          <t>TIMS-151062</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-199419</t>
+          <t>/Road/All/Disruption/TIMS-151062</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[-0.013789,51.529868]</t>
+          <t>[0.00769,51.497244]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -2283,7 +2283,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>[A118] High Street (All approaches) at the junction of [A11] Bow Road - Lane closures on all approaches and on the roundabout, and closure of the link road under the flyover due to Sivertown Tunnel works.</t>
+          <t>Silvertown Tunnel project, Greenwich Peninsula - Various restrictions during Silvertown Tunnel-related works until 2025. Millennium Way is currently closed. There are associated lane closures on the northbound A102 Blackwall Tunnel Southern Approach. https://tfl.gov.uk/travel-information/improvements-and-projects/silvertown-tunnel for More information.</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-01-22T13:57:59Z</t>
+          <t>2025-01-22T09:28:23Z</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -2303,17 +2303,17 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>2024-09-09T06:00:00Z</t>
+          <t>2022-02-25T06:00:00Z</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>2025-02-28T18:00:00Z</t>
+          <t>2025-02-28T19:00:00Z</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>2025-01-22T13:57:59Z</t>
+          <t>2025-01-22T09:28:35Z</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>[A118] HIGH STREET (E15,E3) (Newham,Tower Hamlets)</t>
+          <t>Silvertown Tunnel, Greenwich Peninsula () ()</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.013789, 51.529868], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [0.00769, 51.497244], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T16" t="b">
@@ -2357,8 +2357,16 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>{'type': 'Polygon', 'coordinates': [[[0.0015872809, 51.4994855395], [0.0015897148, 51.4992666821], [0.0016885753, 51.4988833813], [0.0016314069, 51.4987285591], [0.0016568367, 51.4985866611], [0.0019712238, 51.4979597667], [0.0023367167, 51.4975643625], [0.0025422294, 51.497405737], [0.0027389749, 51.4973212985], [0.0028857986, 51.4971786154], [0.0032817226, 51.4969679907], [0.0036324947, 51.4968091112], [0.0045402187, 51.4965116836], [0.0051856762, 51.496244657], [0.0064699118, 51.4955260853], [0.0070259249, 51.4951091885], [0.0087940711, 51.4932803599], [0.0089678651, 51.4931566798], [0.0092013205, 51.4930803307], [0.009419017, 51.4930604705], [0.009677711, 51.4930919214], [0.0099009382, 51.4931793818], [0.0101521911, 51.4933494463], [0.0102606547, 51.4934993865], [0.0102704153, 51.4936840902], [0.0101780164, 51.4938381663], [0.0083987027, 51.4956262966], [0.007615656, 51.4962272295], [0.0065322849, 51.4968444697], [0.0058832964, 51.4971475599], [0.0042083911, 51.4977702357], [0.0042727381, 51.498015522], [0.0041219133, 51.4982417511], [0.0038033644, 51.4983849674], [0.0034069352, 51.4984018868], [0.0032000956, 51.4987592312], [0.0030273742, 51.4993663183], [0.0034746141, 51.4992343554], [0.0038570926, 51.4991790843], [0.0045806689, 51.4991983595], [0.0048184572, 51.4989804061], [0.0050274039, 51.4987036001], [0.0055082382, 51.4985043958], [0.0057270621, 51.4984819495], [0.0059363238, 51.4985002166], [0.0063653164, 51.4986623735], [0.0066790105, 51.4981879482], [0.0072353152, 51.4969522704], [0.0074007888, 51.4967382108], [0.0076938923, 51.4964955835], [0.0086199482, 51.4959914803], [0.0087223435, 51.4958369657], [0.0088904924, 51.4957247339], [0.010439352, 51.495108141], [0.0117602581, 51.4944862226], [0.0124703221, 51.494065049], [0.0129738181, 51.4936681131], [0.0137420234, 51.4929661795], [0.0142808171, 51.492603644], [0.0146295168, 51.4924845516], [0.014902636, 51.4924649862], [0.0151675912, 51.4925107526], [0.0154207872, 51.4926418906], [0.015525296, 51.492763034], [0.0155658857, 51.4929327625], [0.0153694386, 51.4932953386], [0.0148972224, 51.4937702397], [0.013715767, 51.494709575], [0.0133671218, 51.4949377313], [0.0127480886, 51.495256675], [0.0114413891, 51.4958763982], [0.0098541975, 51.4965256119], [0.0087599504, 51.4971000836], [0.0086395409, 51.4972004985], [0.0085228769, 51.4973738007], [0.0081991183, 51.4981468108], [0.0079049483, 51.4987108938], [0.0074674791, 51.4993002501], [0.007205435, 51.4995786317], [0.0069721259, 51.4997120679], [0.0066342853, 51.4997713433], [0.0063565283, 51.4997417503], [0.0060107636, 51.4996121336], [0.0049469675, 51.5005086501], [0.0047269485, 51.5006077687], [0.0044948574, 51.5006474759], [0.0044782548, 51.5007908362], [0.0043357538, 51.5010384505], [0.0039530755, 51.5013272797], [0.0035126028, 51.5014767161], [0.0026982065, 51.5015478698], [0.0022173053, 51.5015195921], [0.0020496151, 51.5014707466], [0.0018673555, 51.5013674381], [0.0017515151, 51.5012318473], [0.0016903855, 51.5010556904], [0.0017293418, 51.5006410701], [0.0015872809, 51.4994855395]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'MILLENNIUM WAY (SE10)', 'closure': 'Open', 'directions': 'Southbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005474,51.496777],[0.007099,51.495915]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005474,51.496777],[0.007099,51.495915]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005474,51.496777],[0.007099,51.495915]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005474,51.496777],[0.007099,51.495915]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006994,51.495835],[0.004605,51.496996]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006994,51.495835],[0.004605,51.496996]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006994,51.495835],[0.004605,51.496996]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006994,51.495835],[0.004605,51.496996]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002408,51.501016],[0.002614,51.498426]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002408,51.501016],[0.002614,51.498426]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002408,51.501016],[0.002614,51.498426]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002408,51.501016],[0.002614,51.498426]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008862,51.494086],[0.00805,51.494945]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008862,51.494086],[0.00805,51.494945]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008862,51.494086],[0.00805,51.494945]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008862,51.494086],[0.00805,51.494945]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008304,51.494878],[0.009561,51.493606]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008304,51.494878],[0.009561,51.493606]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008304,51.494878],[0.009561,51.493606]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008304,51.494878],[0.009561,51.493606]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007099,51.495915],[0.008182,51.495006]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007099,51.495915],[0.008182,51.495006]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007099,51.495915],[0.008182,51.495006]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007099,51.495915],[0.008182,51.495006]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00805,51.494945],[0.006994,51.495835]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00805,51.494945],[0.006994,51.495835]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00805,51.494945],[0.006994,51.495835]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00805,51.494945],[0.006994,51.495835]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009413,51.49351],[0.008862,51.494086]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009413,51.49351],[0.008862,51.494086]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009413,51.49351],[0.008862,51.494086]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009413,51.49351],[0.008862,51.494086]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003558,51.497963],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003558,51.497963],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003558,51.497963],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003558,51.497963],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003043,51.497729],[0.002918,51.49783]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003043,51.497729],[0.002918,51.49783]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003043,51.497729],[0.002918,51.49783]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003043,51.497729],[0.002918,51.49783]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003043,51.497729]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003043,51.497729]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003043,51.497729]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003043,51.497729]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003079,51.49789],[0.00319,51.497798]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003079,51.49789],[0.00319,51.497798]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003079,51.49789],[0.00319,51.497798]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003079,51.49789],[0.00319,51.497798]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003388,51.50101],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003388,51.50101],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003388,51.50101],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003388,51.50101],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003375,51.500826],[0.003634,51.500604]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003375,51.500826],[0.003634,51.500604]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003375,51.500826],[0.003634,51.500604]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003375,51.500826],[0.003634,51.500604]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005733,51.498931],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005733,51.498931],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002908,51.500043],[0.002992,51.500921]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002908,51.500043],[0.002992,51.500921]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002908,51.500043],[0.002992,51.500921]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002908,51.500043],[0.002992,51.500921]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.003142,51.50105]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.003142,51.50105]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.003142,51.50105]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.003142,51.50105]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.004778,51.499758]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.004778,51.499758]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.004778,51.499758]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.004778,51.499758]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.002989,51.5001]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.002989,51.5001]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.002989,51.5001]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.002989,51.5001]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.002435,51.501091]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.002435,51.501091]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.002435,51.501091]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.002435,51.501091]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005733,51.498931],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005733,51.498931],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004889,51.499746],[0.005733,51.498931]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004889,51.499746],[0.005733,51.498931]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004889,51.499746],[0.005733,51.498931]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004889,51.499746],[0.005733,51.498931]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003455,51.497596],[0.004594,51.497109]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003455,51.497596],[0.004594,51.497109]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003455,51.497596],[0.004594,51.497109]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003455,51.497596],[0.004594,51.497109]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004605,51.496996],[0.003427,51.497478]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004605,51.496996],[0.003427,51.497478]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004605,51.496996],[0.003427,51.497478]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004605,51.496996],[0.003427,51.497478]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002493,51.498388],[0.002351,51.498707]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002493,51.498388],[0.002351,51.498707]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002493,51.498388],[0.002351,51.498707]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002493,51.498388],[0.002351,51.498707]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004594,51.497109],[0.005474,51.496777]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004594,51.497109],[0.005474,51.496777]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004594,51.497109],[0.005474,51.496777]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004594,51.497109],[0.005474,51.496777]]', 'sourceSystemId': 0}], 'sourceSystemId': 151062, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'WEST PARKSIDE (SE10)', 'closure': 'Open', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006614,51.499322],[0.009429,51.496162]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006614,51.499322],[0.009429,51.496162]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006614,51.499322],[0.009429,51.496162]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006614,51.499322],[0.009429,51.496162]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009429,51.496162],[0.012213,51.494946]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009429,51.496162],[0.012213,51.494946]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009429,51.496162],[0.012213,51.494946]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009429,51.496162],[0.012213,51.494946]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012312,51.494899],[0.014628,51.493201]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012312,51.494899],[0.014628,51.493201]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012312,51.494899],[0.014628,51.493201]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012312,51.494899],[0.014628,51.493201]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.01211,51.494884],[0.009949,51.495839]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.01211,51.494884],[0.009949,51.495839]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.01211,51.494884],[0.009949,51.495839]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.01211,51.494884],[0.009949,51.495839]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.013837,51.493662],[0.012226,51.49483]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.013837,51.493662],[0.012226,51.49483]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.013837,51.493662],[0.012226,51.49483]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.013837,51.493662],[0.012226,51.49483]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012213,51.494946],[0.012312,51.494899]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012213,51.494946],[0.012312,51.494899]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012213,51.494946],[0.012312,51.494899]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012213,51.494946],[0.012312,51.494899]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012226,51.49483],[0.01211,51.494884]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012226,51.49483],[0.01211,51.494884]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012226,51.49483],[0.01211,51.494884]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012226,51.49483],[0.01211,51.494884]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009325,51.496083],[0.007957,51.496849]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007453,51.497774],[0.006482,51.49927]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007453,51.497774],[0.006482,51.49927]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007453,51.497774],[0.006482,51.49927]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid':</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2368,17 +2376,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>TIMS-205721</t>
+          <t>TIMS-199419</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205721</t>
+          <t>/Road/All/Disruption/TIMS-199419</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>[-0.287669,51.553499]</t>
+          <t>[-0.013789,51.529868]</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -2396,22 +2404,22 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Borough works</t>
+          <t>TfL works</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>[A404] High Road (Both directions) at the junction of [B4565] Wembley Hill Road - Temporary traffic signals in place to facilitate roadworks.</t>
+          <t>[A118] High Street (All approaches) at the junction of [A11] Bow Road - Lane closures on all approaches and on the roundabout, and closure of the link road under the flyover due to Sivertown Tunnel works.</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>There are no reported delays</t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-01-22T20:35:13Z</t>
+          <t>2025-01-22T13:57:59Z</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -2421,17 +2429,17 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>2025-01-13T05:00:00Z</t>
+          <t>2024-09-09T06:00:00Z</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2025-05-19T17:00:00Z</t>
+          <t>2025-02-28T18:00:00Z</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>2025-01-22T20:35:13Z</t>
+          <t>2025-01-22T13:57:59Z</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -2441,7 +2449,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>[A404] HIGH ROAD (HA9) (Brent)</t>
+          <t>[A118] HIGH STREET (E15,E3) (Newham,Tower Hamlets)</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -2451,7 +2459,7 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.287669, 51.553499], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.013789, 51.529868], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T17" t="b">
@@ -2486,17 +2494,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>TIMS-151062</t>
+          <t>TIMS-200121</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-151062</t>
+          <t>/Road/All/Disruption/TIMS-200121</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>[0.00769,51.497244]</t>
+          <t>[-0.008204,51.507309]</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2519,7 +2527,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Silvertown Tunnel project, Greenwich Peninsula - Various restrictions during Silvertown Tunnel-related works until 2025. Millennium Way is currently closed. There are associated lane closures on the northbound A102 Blackwall Tunnel Southern Approach. https://tfl.gov.uk/travel-information/improvements-and-projects/silvertown-tunnel for More information.</t>
+          <t>Silvertown Tunnel Scheme - Preston's Roundabout - [A1206] Prestons Road Roundabout (All directions) between [A1206] Prestons Road and [A1261] Aspen Way - Lane restrictions are in place to facilitate Silvertown Tunnel related works.</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -2529,7 +2537,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-01-22T09:28:23Z</t>
+          <t>2025-01-22T13:38:22Z</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -2539,17 +2547,17 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>2022-02-25T06:00:00Z</t>
+          <t>2024-09-16T06:00:00Z</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>2025-02-28T19:00:00Z</t>
+          <t>2025-03-01T19:00:00Z</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>2025-01-22T09:28:35Z</t>
+          <t>2025-01-22T13:38:22Z</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -2559,7 +2567,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>Silvertown Tunnel, Greenwich Peninsula () ()</t>
+          <t>[A1206] PRESTONS ROAD ROUNDABOUT (E14) (Tower Hamlets)</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -2569,7 +2577,7 @@
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [0.00769, 51.497244], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.008204, 51.507309], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T18" t="b">
@@ -2593,16 +2601,8 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y18" t="inlineStr">
-        <is>
-          <t>{'type': 'Polygon', 'coordinates': [[[0.0015872809, 51.4994855395], [0.0015897148, 51.4992666821], [0.0016885753, 51.4988833813], [0.0016314069, 51.4987285591], [0.0016568367, 51.4985866611], [0.0019712238, 51.4979597667], [0.0023367167, 51.4975643625], [0.0025422294, 51.497405737], [0.0027389749, 51.4973212985], [0.0028857986, 51.4971786154], [0.0032817226, 51.4969679907], [0.0036324947, 51.4968091112], [0.0045402187, 51.4965116836], [0.0051856762, 51.496244657], [0.0064699118, 51.4955260853], [0.0070259249, 51.4951091885], [0.0087940711, 51.4932803599], [0.0089678651, 51.4931566798], [0.0092013205, 51.4930803307], [0.009419017, 51.4930604705], [0.009677711, 51.4930919214], [0.0099009382, 51.4931793818], [0.0101521911, 51.4933494463], [0.0102606547, 51.4934993865], [0.0102704153, 51.4936840902], [0.0101780164, 51.4938381663], [0.0083987027, 51.4956262966], [0.007615656, 51.4962272295], [0.0065322849, 51.4968444697], [0.0058832964, 51.4971475599], [0.0042083911, 51.4977702357], [0.0042727381, 51.498015522], [0.0041219133, 51.4982417511], [0.0038033644, 51.4983849674], [0.0034069352, 51.4984018868], [0.0032000956, 51.4987592312], [0.0030273742, 51.4993663183], [0.0034746141, 51.4992343554], [0.0038570926, 51.4991790843], [0.0045806689, 51.4991983595], [0.0048184572, 51.4989804061], [0.0050274039, 51.4987036001], [0.0055082382, 51.4985043958], [0.0057270621, 51.4984819495], [0.0059363238, 51.4985002166], [0.0063653164, 51.4986623735], [0.0066790105, 51.4981879482], [0.0072353152, 51.4969522704], [0.0074007888, 51.4967382108], [0.0076938923, 51.4964955835], [0.0086199482, 51.4959914803], [0.0087223435, 51.4958369657], [0.0088904924, 51.4957247339], [0.010439352, 51.495108141], [0.0117602581, 51.4944862226], [0.0124703221, 51.494065049], [0.0129738181, 51.4936681131], [0.0137420234, 51.4929661795], [0.0142808171, 51.492603644], [0.0146295168, 51.4924845516], [0.014902636, 51.4924649862], [0.0151675912, 51.4925107526], [0.0154207872, 51.4926418906], [0.015525296, 51.492763034], [0.0155658857, 51.4929327625], [0.0153694386, 51.4932953386], [0.0148972224, 51.4937702397], [0.013715767, 51.494709575], [0.0133671218, 51.4949377313], [0.0127480886, 51.495256675], [0.0114413891, 51.4958763982], [0.0098541975, 51.4965256119], [0.0087599504, 51.4971000836], [0.0086395409, 51.4972004985], [0.0085228769, 51.4973738007], [0.0081991183, 51.4981468108], [0.0079049483, 51.4987108938], [0.0074674791, 51.4993002501], [0.007205435, 51.4995786317], [0.0069721259, 51.4997120679], [0.0066342853, 51.4997713433], [0.0063565283, 51.4997417503], [0.0060107636, 51.4996121336], [0.0049469675, 51.5005086501], [0.0047269485, 51.5006077687], [0.0044948574, 51.5006474759], [0.0044782548, 51.5007908362], [0.0043357538, 51.5010384505], [0.0039530755, 51.5013272797], [0.0035126028, 51.5014767161], [0.0026982065, 51.5015478698], [0.0022173053, 51.5015195921], [0.0020496151, 51.5014707466], [0.0018673555, 51.5013674381], [0.0017515151, 51.5012318473], [0.0016903855, 51.5010556904], [0.0017293418, 51.5006410701], [0.0015872809, 51.4994855395]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="Z18" t="inlineStr">
-        <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'MILLENNIUM WAY (SE10)', 'closure': 'Open', 'directions': 'Southbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005474,51.496777],[0.007099,51.495915]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005474,51.496777],[0.007099,51.495915]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005474,51.496777],[0.007099,51.495915]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005474,51.496777],[0.007099,51.495915]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006994,51.495835],[0.004605,51.496996]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006994,51.495835],[0.004605,51.496996]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006994,51.495835],[0.004605,51.496996]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006994,51.495835],[0.004605,51.496996]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002408,51.501016],[0.002614,51.498426]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002408,51.501016],[0.002614,51.498426]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002408,51.501016],[0.002614,51.498426]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002408,51.501016],[0.002614,51.498426]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008862,51.494086],[0.00805,51.494945]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008862,51.494086],[0.00805,51.494945]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008862,51.494086],[0.00805,51.494945]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008862,51.494086],[0.00805,51.494945]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008304,51.494878],[0.009561,51.493606]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008304,51.494878],[0.009561,51.493606]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008304,51.494878],[0.009561,51.493606]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.008304,51.494878],[0.009561,51.493606]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007099,51.495915],[0.008182,51.495006]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007099,51.495915],[0.008182,51.495006]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007099,51.495915],[0.008182,51.495006]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007099,51.495915],[0.008182,51.495006]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00805,51.494945],[0.006994,51.495835]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00805,51.494945],[0.006994,51.495835]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00805,51.494945],[0.006994,51.495835]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00805,51.494945],[0.006994,51.495835]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009413,51.49351],[0.008862,51.494086]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009413,51.49351],[0.008862,51.494086]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009413,51.49351],[0.008862,51.494086]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009413,51.49351],[0.008862,51.494086]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003558,51.497963],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003558,51.497963],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003558,51.497963],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003558,51.497963],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003455,51.497596]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003043,51.497729],[0.002918,51.49783]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003043,51.497729],[0.002918,51.49783]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003043,51.497729],[0.002918,51.49783]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003043,51.497729],[0.002918,51.49783]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003043,51.497729]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003043,51.497729]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003043,51.497729]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.00319,51.497798],[0.003043,51.497729]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003079,51.49789],[0.00319,51.497798]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003079,51.49789],[0.00319,51.497798]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003079,51.49789],[0.00319,51.497798]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003079,51.49789],[0.00319,51.497798]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003388,51.50101],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003388,51.50101],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003388,51.50101],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003388,51.50101],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003375,51.500826],[0.003634,51.500604]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003375,51.500826],[0.003634,51.500604]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003375,51.500826],[0.003634,51.500604]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003375,51.500826],[0.003634,51.500604]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005733,51.498931],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005733,51.498931],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.003388,51.50101]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002908,51.500043],[0.002992,51.500921]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002908,51.500043],[0.002992,51.500921]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002908,51.500043],[0.002992,51.500921]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002908,51.500043],[0.002992,51.500921]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.003142,51.50105]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.003142,51.50105]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.003142,51.50105]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.003142,51.50105]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003634,51.500604],[0.003375,51.500826]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.004778,51.499758]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.004778,51.499758]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.004778,51.499758]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002989,51.5001],[0.004778,51.499758]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.002989,51.5001]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.002989,51.5001]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.002989,51.5001]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002992,51.500921],[0.002989,51.5001]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.002435,51.501091]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.002435,51.501091]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.002435,51.501091]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003142,51.50105],[0.002435,51.501091]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004778,51.499758],[0.004889,51.499746]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005733,51.498931],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.005733,51.498931],[0.002908,51.500043]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004889,51.499746],[0.005733,51.498931]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004889,51.499746],[0.005733,51.498931]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004889,51.499746],[0.005733,51.498931]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004889,51.499746],[0.005733,51.498931]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003455,51.497596],[0.004594,51.497109]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003455,51.497596],[0.004594,51.497109]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003455,51.497596],[0.004594,51.497109]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.003455,51.497596],[0.004594,51.497109]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004605,51.496996],[0.003427,51.497478]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004605,51.496996],[0.003427,51.497478]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004605,51.496996],[0.003427,51.497478]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004605,51.496996],[0.003427,51.497478]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002918,51.49783],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002493,51.498388],[0.002351,51.498707]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002493,51.498388],[0.002351,51.498707]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002493,51.498388],[0.002351,51.498707]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002493,51.498388],[0.002351,51.498707]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.002493,51.498388]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.002614,51.498426],[0.003079,51.49789]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004594,51.497109],[0.005474,51.496777]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004594,51.497109],[0.005474,51.496777]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004594,51.497109],[0.005474,51.496777]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.004594,51.497109],[0.005474,51.496777]]', 'sourceSystemId': 0}], 'sourceSystemId': 151062, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'WEST PARKSIDE (SE10)', 'closure': 'Open', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006614,51.499322],[0.009429,51.496162]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006614,51.499322],[0.009429,51.496162]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006614,51.499322],[0.009429,51.496162]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.006614,51.499322],[0.009429,51.496162]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009429,51.496162],[0.012213,51.494946]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009429,51.496162],[0.012213,51.494946]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009429,51.496162],[0.012213,51.494946]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009429,51.496162],[0.012213,51.494946]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012312,51.494899],[0.014628,51.493201]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012312,51.494899],[0.014628,51.493201]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012312,51.494899],[0.014628,51.493201]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012312,51.494899],[0.014628,51.493201]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.01211,51.494884],[0.009949,51.495839]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.01211,51.494884],[0.009949,51.495839]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.01211,51.494884],[0.009949,51.495839]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.01211,51.494884],[0.009949,51.495839]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.013837,51.493662],[0.012226,51.49483]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.013837,51.493662],[0.012226,51.49483]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.013837,51.493662],[0.012226,51.49483]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.013837,51.493662],[0.012226,51.49483]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012213,51.494946],[0.012312,51.494899]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012213,51.494946],[0.012312,51.494899]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012213,51.494946],[0.012312,51.494899]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012213,51.494946],[0.012312,51.494899]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012226,51.49483],[0.01211,51.494884]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012226,51.49483],[0.01211,51.494884]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012226,51.49483],[0.01211,51.494884]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.012226,51.49483],[0.01211,51.494884]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.009325,51.496083],[0.007957,51.496849]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007453,51.497774],[0.006482,51.49927]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007453,51.497774],[0.006482,51.49927]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[0.007453,51.497774],[0.006482,51.49927]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid':</t>
-        </is>
-      </c>
+      <c r="Y18" t="inlineStr"/>
+      <c r="Z18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2612,17 +2612,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>TIMS-206169</t>
+          <t>TIMS-205922</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206169</t>
+          <t>/Road/All/Disruption/TIMS-205922</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[0.107786,51.533152]</t>
+          <t>[-0.113322,51.521519]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -2635,47 +2635,47 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Breakdowns</t>
+          <t>Works</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Vehicle breakdown</t>
+          <t>Borough works</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>[A13] Ripple Road (Eastbound) at the junction of [A1153] Lodge Avenue - Lane two (of two) is blocked due to a broken down car</t>
+          <t>[A5200] Grays Inn Road (Southbound) at the junction of [A5201] Clerkenwell Road - Lane closures to facilitate Local Authority improvement works.</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Approach with caution. </t>
+          <t>Use an alternative route. There are no reported delays on diversion.</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-01-22T20:37:15Z</t>
+          <t>2025-01-22T20:50:00Z</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>['a13']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2025-01-22T19:26:03Z</t>
+          <t>2025-01-15T19:50:33Z</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>2025-01-22T23:59:59Z</t>
+          <t>2025-01-15T23:59:59Z</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>2025-01-22T20:37:15Z</t>
+          <t>2025-01-22T20:50:00Z</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>[A13] RIPPLE ROAD (IG11,RM9) (Barking &amp; Dagenham)</t>
+          <t>[A5200] GRAYS INN ROAD (EC1N,WC1N,WC1R,WC1X) (Camden)</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2695,7 +2695,7 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [0.107786, 51.533152], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.113322, 51.521519], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T19" t="b">
@@ -2719,8 +2719,16 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y19" t="inlineStr"/>
-      <c r="Z19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>{'type': 'Polygon', 'coordinates': [[[-0.1140419035, 51.5215119215], [-0.1139958498, 51.52136097], [-0.1128170679, 51.5195291901], [-0.1119393265, 51.5179543006], [-0.11177142, 51.5178204921], [-0.1115358794, 51.5177351471], [-0.1112663842, 51.517710469], [-0.110970608, 51.5177592556], [-0.1107558744, 51.5178638044], [-0.1106187171, 51.5180106237], [-0.110578092, 51.5181573554], [-0.1106219388, 51.5184036666], [-0.1116986267, 51.5202238788], [-0.1126876468, 51.5217326452], [-0.1128399582, 51.5218534079], [-0.1129923936, 51.5219189533], [-0.1132275053, 51.5219647778], [-0.1134736201, 51.5219585112], [-0.1137019633, 51.5219008864], [-0.1138858377, 51.5217986405], [-0.114003746, 51.5216637278], [-0.1140419035, 51.5215119215]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A5200] GRAYS INN ROAD (EC1N,WC1R,WC1X)', 'closure': 'Closed', 'directions': 'Southbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.111341,51.518251],[-0.111298,51.518159]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.111681,51.518868],[-0.11141,51.518396]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.11141,51.518396],[-0.111341,51.518251]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.11214,51.519683],[-0.111681,51.518868]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.112509,51.520256],[-0.11214,51.519683]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.112794,51.520683],[-0.112509,51.520256]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.113322,51.521519],[-0.112794,51.520683]]', 'sourceSystemId': 0}], 'sourceSystemId': 205922, 'sourceSystemKey': 'TIMS'}]</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2730,22 +2738,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>TIMS-205922</t>
+          <t>TIMS-205882</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205922</t>
+          <t>/Road/All/Disruption/TIMS-205882</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>[-0.113322,51.521519]</t>
+          <t>[-0.063901,51.589292]</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Minimal</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -2758,42 +2766,42 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Borough works</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>[A5200] Grays Inn Road (Southbound) at the junction of [A5201] Clerkenwell Road - Lane closures to facilitate Local Authority improvement works.</t>
+          <t xml:space="preserve">[A503] Monument Way (Westbound) at the junction of [A1055] The Hale - Lane restrictions westbound to facilitate electrical cable placement works. </t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Use an alternative route. There are no reported delays on diversion.</t>
+          <t xml:space="preserve">Delays are possible. </t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-01-22T20:50:00Z</t>
+          <t>2025-01-22T08:21:58Z</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['a10']</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>2025-01-15T19:50:33Z</t>
+          <t>2025-01-15T02:30:00Z</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>2025-01-15T23:59:59Z</t>
+          <t>2025-01-26T17:00:00Z</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>2025-01-22T20:50:00Z</t>
+          <t>2025-01-22T08:22:08Z</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2803,7 +2811,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>[A5200] GRAYS INN ROAD (EC1N,WC1N,WC1R,WC1X) (Camden)</t>
+          <t>[A503] MONUMENT WAY (N15,N17) (Haringey)</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2813,7 +2821,7 @@
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.113322, 51.521519], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.063901, 51.589292], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T20" t="b">
@@ -2837,16 +2845,8 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y20" t="inlineStr">
-        <is>
-          <t>{'type': 'Polygon', 'coordinates': [[[-0.1140419035, 51.5215119215], [-0.1139958498, 51.52136097], [-0.1128170679, 51.5195291901], [-0.1119393265, 51.5179543006], [-0.11177142, 51.5178204921], [-0.1115358794, 51.5177351471], [-0.1112663842, 51.517710469], [-0.110970608, 51.5177592556], [-0.1107558744, 51.5178638044], [-0.1106187171, 51.5180106237], [-0.110578092, 51.5181573554], [-0.1106219388, 51.5184036666], [-0.1116986267, 51.5202238788], [-0.1126876468, 51.5217326452], [-0.1128399582, 51.5218534079], [-0.1129923936, 51.5219189533], [-0.1132275053, 51.5219647778], [-0.1134736201, 51.5219585112], [-0.1137019633, 51.5219008864], [-0.1138858377, 51.5217986405], [-0.114003746, 51.5216637278], [-0.1140419035, 51.5215119215]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="Z20" t="inlineStr">
-        <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A5200] GRAYS INN ROAD (EC1N,WC1R,WC1X)', 'closure': 'Closed', 'directions': 'Southbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.111341,51.518251],[-0.111298,51.518159]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.111681,51.518868],[-0.11141,51.518396]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.11141,51.518396],[-0.111341,51.518251]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.11214,51.519683],[-0.111681,51.518868]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.112509,51.520256],[-0.11214,51.519683]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.112794,51.520683],[-0.112509,51.520256]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.113322,51.521519],[-0.112794,51.520683]]', 'sourceSystemId': 0}], 'sourceSystemId': 205922, 'sourceSystemKey': 'TIMS'}]</t>
-        </is>
-      </c>
+      <c r="Y20" t="inlineStr"/>
+      <c r="Z20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2856,17 +2856,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>TIMS-205882</t>
+          <t>TIMS-204935</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205882</t>
+          <t>/Road/All/Disruption/TIMS-204935</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>[-0.063901,51.589292]</t>
+          <t>[-0.096374,51.494502]</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2884,12 +2884,12 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>TfL works</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t xml:space="preserve">[A503] Monument Way (Westbound) at the junction of [A1055] The Hale - Lane restrictions westbound to facilitate electrical cable placement works. </t>
+          <t>[A201] New Kent Road (Both directions) between Elephant Road and Balfour Street - Various restrictions to facilitate TfL improvement works. Between 06 January - 22 January, lane closures in both directions. Full westbound closure in place on the nights of 03, 04 March. Full eastbound closure in place on the nights of 04, 05 March.</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2899,27 +2899,27 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-01-22T08:21:58Z</t>
+          <t>2025-01-22T08:07:35Z</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>['a10']</t>
+          <t>['a2', 'inner ring']</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2025-01-15T02:30:00Z</t>
+          <t>2025-01-06T08:00:00Z</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>2025-01-26T17:00:00Z</t>
+          <t>2025-03-06T05:00:00Z</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>2025-01-22T08:22:08Z</t>
+          <t>2025-01-22T08:07:44Z</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>[A503] MONUMENT WAY (N15,N17) (Haringey)</t>
+          <t>[A201] NEW KENT ROAD (SE1,SE17) (Southwark)</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.063901, 51.589292], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.096374, 51.494502], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T21" t="b">
@@ -2974,17 +2974,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>TIMS-206173</t>
+          <t>TIMS-204984</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206173</t>
+          <t>/Road/All/Disruption/TIMS-204984</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[-0.014454,51.529785]</t>
+          <t>[0.01712,51.446785]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -2997,47 +2997,47 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Breakdowns</t>
+          <t>Works</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Vehicle breakdown</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>[A12] Blackwall Tunnel Northern Approach (Eastbound) at the junction of [A11] Bow Road - The roundabout is blocked due to a broken down car</t>
+          <t>[A205] Westhorne Avenue (Both directions) between Baring Road and (A20) Sidcup Road - Lane restrictions are in place to facilitate Thames Water works.</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Use other route.</t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-01-22T20:12:43Z</t>
+          <t>2025-01-22T09:27:38Z</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>['a12', 'blackwall tunnel']</t>
+          <t>['a205']</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>2025-01-22T20:01:10Z</t>
+          <t>2024-12-19T10:00:00Z</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>2025-01-22T23:59:59Z</t>
+          <t>2025-04-07T17:00:00Z</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>2025-01-22T20:41:29Z</t>
+          <t>2025-01-22T09:27:47Z</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -3047,7 +3047,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>[A12] BLACKWALL TUNNEL NORTHERN APPROACH (E14,E15,E3) (Tower Hamlets)</t>
+          <t>[A205] WESTHORNE AVENUE (SE12) (Greenwich,Lewisham)</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.014454, 51.529785], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [0.01712, 51.446785], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T22" t="b">
@@ -3092,17 +3092,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>TIMS-204935</t>
+          <t>TIMS-205984</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204935</t>
+          <t>/Road/All/Disruption/TIMS-205984</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>[-0.096374,51.494502]</t>
+          <t>[-0.162149,51.434329]</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -3120,42 +3120,42 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>TfL works</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>[A201] New Kent Road (Both directions) between Elephant Road and Balfour Street - Various restrictions to facilitate TfL improvement works. Between 06 January - 22 January, lane closures in both directions. Full westbound closure in place on the nights of 03, 04 March. Full eastbound closure in place on the nights of 04, 05 March.</t>
+          <t>[A24] Upper Tooting Road (Both directions) at the junction of Beechcroft Road - Single alternate lane operated by temporary signals for utility works.</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delays are possible. </t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-01-22T08:07:35Z</t>
+          <t>2025-01-22T09:37:48Z</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>['a2', 'inner ring']</t>
+          <t>['a24']</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>2025-01-06T08:00:00Z</t>
+          <t>2025-01-17T04:30:00Z</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>2025-03-06T05:00:00Z</t>
+          <t>2025-01-26T18:00:00Z</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>2025-01-22T08:07:44Z</t>
+          <t>2025-01-22T09:37:48Z</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -3165,7 +3165,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>[A201] NEW KENT ROAD (SE1,SE17) (Southwark)</t>
+          <t>[A24] UPPER TOOTING ROAD (SW17) (Wandsworth)</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -3175,7 +3175,7 @@
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.096374, 51.494502], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.162149, 51.434329], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T23" t="b">
@@ -3210,17 +3210,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>TIMS-204984</t>
+          <t>TIMS-204983</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204984</t>
+          <t>/Road/All/Disruption/TIMS-204983</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>[0.01712,51.446785]</t>
+          <t>[-0.330213,51.455737]</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -3238,12 +3238,12 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>TfL works</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>[A205] Westhorne Avenue (Both directions) between Baring Road and (A20) Sidcup Road - Lane restrictions are in place to facilitate Thames Water works.</t>
+          <t xml:space="preserve">[A316] Chertsey Road (Both directions) at the junction of [A310] London Road - There are lane restrictions in place due to junction improvement works. </t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -3253,12 +3253,12 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-01-22T09:27:38Z</t>
+          <t>2025-01-22T09:35:19Z</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>['a205']</t>
+          <t>['a316']</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -3268,12 +3268,12 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>2025-04-07T17:00:00Z</t>
+          <t>2025-07-25T04:00:00Z</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>2025-01-22T09:27:47Z</t>
+          <t>2025-01-22T09:35:32Z</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -3283,7 +3283,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>[A205] WESTHORNE AVENUE (SE12) (Greenwich,Lewisham)</t>
+          <t>[A316] CHERTSEY ROAD (TW1,TW2) (Richmond upon Thames)</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -3293,7 +3293,7 @@
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [0.01712, 51.446785], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.330213, 51.455737], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T24" t="b">
@@ -3328,17 +3328,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>TIMS-205984</t>
+          <t>TIMS-206084</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205984</t>
+          <t>/Road/All/Disruption/TIMS-206084</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[-0.162149,51.434329]</t>
+          <t>[-0.297428,51.465248]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -3361,37 +3361,37 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>[A24] Upper Tooting Road (Both directions) at the junction of Beechcroft Road - Single alternate lane operated by temporary signals for utility works.</t>
+          <t>[A316] Lower Mortlake Road (Westbound) at the junction of Salisbury Road - Lane one of two is closed to facilitate Cadent Gas works.</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-01-22T09:37:48Z</t>
+          <t>2025-01-22T19:08:26Z</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>['a24']</t>
+          <t>['a316']</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>2025-01-17T04:30:00Z</t>
+          <t>2025-01-20T15:26:00Z</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>2025-01-26T18:00:00Z</t>
+          <t>2025-01-24T23:59:00Z</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>2025-01-22T09:37:48Z</t>
+          <t>2025-01-22T19:08:26Z</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>[A24] UPPER TOOTING ROAD (SW17) (Wandsworth)</t>
+          <t>[A316] LOWER MORTLAKE ROAD (TW9) (Richmond upon Thames)</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -3411,7 +3411,7 @@
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.162149, 51.434329], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.297428, 51.465248], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T25" t="b">
@@ -3446,17 +3446,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>TIMS-204983</t>
+          <t>TIMS-182512</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204983</t>
+          <t>/Road/All/Disruption/TIMS-182512</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>[-0.330213,51.455737]</t>
+          <t>[-0.221082,51.51375]</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -3479,37 +3479,37 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t xml:space="preserve">[A316] Chertsey Road (Both directions) at the junction of [A310] London Road - There are lane restrictions in place due to junction improvement works. </t>
+          <t>A40 Westway Refurbishment Scheme - A3220 West Cross Route - [A3220] West Cross Route (Southbound) between A40 Westway and Ariel Way - A40 Westway eastbound off-slip to Northern Roundabout remains closed. From Monday 2 September until Saturday 12 October, West Cross Route northbound and the slip road to Wood Lane will be closed.</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t>Delays are possible</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-01-22T09:35:19Z</t>
+          <t>2025-01-22T08:18:57Z</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>['a316']</t>
+          <t>['a40', 'western cross route']</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>2024-12-19T10:00:00Z</t>
+          <t>2024-07-21T19:00:00Z</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>2025-07-25T04:00:00Z</t>
+          <t>2025-06-28T17:00:00Z</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>2025-01-22T09:35:32Z</t>
+          <t>2025-01-22T08:18:58Z</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -3519,7 +3519,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>[A316] CHERTSEY ROAD (TW1,TW2) (Richmond upon Thames)</t>
+          <t>[A3220] WEST CROSS ROUTE (W10,W11,W12) (Hammersmith &amp; Fulham,Kensington &amp; Chelsea)</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -3529,7 +3529,7 @@
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.330213, 51.455737], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.221082, 51.51375], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T26" t="b">
@@ -3553,8 +3553,16 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y26" t="inlineStr"/>
-      <c r="Z26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>{'type': 'Polygon', 'coordinates': [[[-0.2268504991, 51.515214368], [-0.226816068, 51.5150759665], [-0.2266923055, 51.5149322348], [-0.2264944531, 51.5148255447], [-0.22624859, 51.514769959], [-0.2222289851, 51.5150082855], [-0.2221113839, 51.5148973036], [-0.2218935207, 51.5147814334], [-0.2217342167, 51.5146209077], [-0.2217165117, 51.5145590974], [-0.2219898415, 51.5142281809], [-0.2221301141, 51.5139454523], [-0.2221449065, 51.5138085631], [-0.2220721873, 51.5134910081], [-0.2205678856, 51.5111075751], [-0.2202148706, 51.5103339389], [-0.2198150378, 51.5091676116], [-0.219675534, 51.5090076612], [-0.2194415557, 51.5088941611], [-0.219086057, 51.5078415649], [-0.2185897904, 51.5066539009], [-0.2182414931, 51.5060381507], [-0.2173647255, 51.5048234777], [-0.2172272759, 51.504723302], [-0.2170491482, 51.5046523398], [-0.2168456828, 51.5046167021], [-0.2166344017, 51.5046194581], [-0.2163718851, 51.5046819683], [-0.2161676828, 51.5048024144], [-0.2160458612, 51.5049840778], [-0.2160517337, 51.5051593879], [-0.2162922472, 51.5055614647], [-0.2169077501, 51.5063788767], [-0.2174019457, 51.507321224], [-0.2186336527, 51.5107487541], [-0.2188885584, 51.5113469276], [-0.2192122199, 51.5118264977], [-0.2200716324, 51.5139055816], [-0.2201046988, 51.5140623912], [-0.2200137181, 51.5143839594], [-0.2195736429, 51.5148589248], [-0.2195083826, 51.515117759], [-0.2174597629, 51.5152667541], [-0.2164061948, 51.5154031442], [-0.2158660738, 51.5155028114], [-0.215089151, 51.5157160863], [-0.2119022877, 51.5168006338], [-0.2085686825, 51.5175740516], [-0.2081537913, 51.5176956104], [-0.2073044872, 51.5179999791], [-0.206542063, 51.5183931404], [-0.2059257385, 51.5187789312], [-0.2042932064, 51.5200279103], [-0.2035689067, 51.5204350978], [-0.2032427421, 51.5205820065], [-0.2025200333, 51.5208331967], [-0.2016527864, 51.5210280674], [-0.2011710714, 51.5210932856], [-0.2001367564, 51.5211473219], [-0.1993063778, 51.5210932442], [-0.1986305215, 51.5209980488], [-0.1977979222, 51.5207917816], [-0.1944017809, 51.5197558416], [-0.1936473833, 51.5195739804], [-0.1927795272, 51.5194060024], [-0.1912417461, 51.519189227], [-0.1900168103, 51.5191038861], [-0.1848656155, 51.5190371619], [-0.1845973629, 51.5190895], [-0.1843816324, 51.5192018967], [-0.1842421283, 51.5193785497], [-0.1842307399, 51.5195537531], [-0.1843099996, 51.5196992406], [-0.184437376, 51.519804493], [-0.1846082423, 51.519882146], [-0.1848427707, 51.5199290971], [-0.1899539586, 51.5200020012], [-0.1910275156, 51.5200785533], [-0.1917208959, 51.5201644808], [-0.192967492, 51.5203817851], [-0.1938615219, 51.5205891585], [-0.1971821776, 51.5216043926], [-0.1982276319, 51.5218612247], [-0.1990755076, 51.5219805605], [-0.2000396338, 51.5220444521], [-0.2012151975, 51.5220008809], [-0.2020360143, 51.5218950351], [-0.2030802769, 51.5216616773], [-0.2040030068, 51.5213458102], [-0.2044268186, 51.5211572666], [-0.2049988503, 51.5208578957], [-0.2056305823, 51.5204459626], [-0.207001595, 51.5193777412], [-0.2076748052, 51.5189613218], [-0.2081285965, 51.5187382039], [-0.2084824166, 51.5186038176], [-0.20911363, 51.5184067448], [-0.2124946693, 51.5176200575], [-0.2132845634, 51.5173738454], [-0.2157446367, 51.5165166288], [-0.2163624004, 51.5163475389], [-0.2176701507, 51.5161561474], [-0.2213144853, 51.5158933476], [-0.2215298893, 51.5159391065], [-0.2217236504, 51.51594327], [-0.2262646465, 51.5156547616], [-0.2264817636, 51.5156054962], [-0.2266844629, 51.5155002741], [-0.2268128844, 51.5153565877], [-0.2268504991, 51.515214368]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+        </is>
+      </c>
+      <c r="Z26" t="inlineStr">
+        <is>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A40] WESTWAY (W10,W12)', 'closure': 'Open', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.22613,51.515213],[-0.224382,51.515322]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.22246,51.515445],[-0.221651,51.515496]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.224382,51.515322],[-0.22246,51.515445]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A40] WESTWAY (W10,W12)', 'closure': 'Closed', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.22613,51.515213],[-0.224382,51.515322]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.22246,51.515445],[-0.221651,51.515496]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.224382,51.515322],[-0.22246,51.515445]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3220] WEST CROSS ROUTE (W10,W11,W12)', 'closure': 'Open', 'directions': 'Southbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.221122,51.514298],[-0.221294,51.51505]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.221294,51.51505],[-0.221576,51.515198]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219205,51.509571],[-0.220102,51.511615]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219126,51.509298],[-0.219205,51.509571]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.220102,51.511615],[-0.221122,51.514298]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3220] WEST CROSS ROUTE (W10,W11,W12)', 'closure': 'Open', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.218945,51.509605],[-0.218851,51.509321]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.218851,51.509321],[-0.218825,51.509249]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.218825,51.509249],[-0.217898,51.50678]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.220227,51.51509],[-0.221294,51.51505]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.220227,51.51509],[-0.219897,51.511684]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.217581,51.506219],[-0.216755,51.505063]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.217898,51.50678],[-0.217581,51.506219]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219897,51.511684],[-0.218945,51.509605]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.221294,51.51505],[-0.221576,51.515198]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3220] WEST CROSS ROUTE (W10,W11,W12)', 'closure': 'Open', 'directions': 'Southbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.221122,51.514298],[-0.221294,51.51505]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.221294,51.51505],[-0.221576,51.515198]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219205,51.509571],[-0.220102,51.511615]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219126,51.509298],[-0.219205,51.509571]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.220102,51.511615],[-0.221122,51.514298]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A40] WESTWAY (W10,W11,W2,W9)', 'closure': 'Open', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.18876,51.519534],[-0.189999,51.519553]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.184942,51.519484],[-0.18876,51.519534]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.216796,51.515809],[-0.21755,51.515713]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.189999,51.519553],[-0.201091,51.521558]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219906,51.515542],[-0.22164,51.515415]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.21372,51.516707],[-0.216796,51.515809]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.21755,51.515713],[-0.219906,51.515542]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.207202,51.518621],[-0.210223,51.517678]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.201091,51.521558],[-0.207202,51.518621]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.210223,51.517678],[-0.21372,51.516707]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}]</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3564,17 +3572,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>TIMS-206084</t>
+          <t>TIMS-205670</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206084</t>
+          <t>/Road/All/Disruption/TIMS-205670</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>[-0.297428,51.465248]</t>
+          <t>[-0.138828,51.524968]</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -3592,42 +3600,42 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>Borough works</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>[A316] Lower Mortlake Road (Westbound) at the junction of Salisbury Road - Lane one of two is closed to facilitate Cadent Gas works.</t>
+          <t>[A501] Euston Road (Eastbound) at the junction of [A400] Hampstead Road - Eastbound footway and carriageway restrictions during Euston Tower Development. Lane 1 of 3 will be closed. From 31/01 - 04/03 northbound lane 1 (of 2) is closed.</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Traffic is flowing well.</t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-01-22T19:08:26Z</t>
+          <t>2025-01-22T08:08:40Z</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>['a316']</t>
+          <t>['inner ring']</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>2025-01-20T15:26:00Z</t>
+          <t>2025-01-09T08:00:00Z</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>2025-01-24T23:59:00Z</t>
+          <t>2025-03-07T18:00:00Z</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>2025-01-22T19:08:26Z</t>
+          <t>2025-01-22T08:08:48Z</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -3637,7 +3645,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>[A316] LOWER MORTLAKE ROAD (TW9) (Richmond upon Thames)</t>
+          <t>[A501] EUSTON ROAD (NW1,WC1H) (Camden,Westminster)</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -3647,7 +3655,7 @@
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.297428, 51.465248], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.138828, 51.524968], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T27" t="b">
@@ -3682,17 +3690,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>TIMS-182512</t>
+          <t>TIMS-204885</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-182512</t>
+          <t>/Road/All/Disruption/TIMS-204885</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>[-0.221082,51.51375]</t>
+          <t>[-0.169931,51.478281]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -3715,37 +3723,37 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>A40 Westway Refurbishment Scheme - A3220 West Cross Route - [A3220] West Cross Route (Southbound) between A40 Westway and Ariel Way - A40 Westway eastbound off-slip to Northern Roundabout remains closed. From Monday 2 September until Saturday 12 October, West Cross Route northbound and the slip road to Wood Lane will be closed.</t>
+          <t>[A3220] Battersea Bridge Road (Both directions) at the junction of Parkgate Road - Lane closure in place to facilitate Urban Realm Works.</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Delays are possible</t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-01-22T08:18:57Z</t>
+          <t>2025-01-22T08:53:58Z</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>['a40', 'western cross route']</t>
+          <t>['western cross route']</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>2024-07-21T19:00:00Z</t>
+          <t>2025-01-20T07:00:00Z</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>2025-06-28T17:00:00Z</t>
+          <t>2025-05-22T06:00:00Z</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>2025-01-22T08:18:58Z</t>
+          <t>2025-01-22T08:53:58Z</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -3755,7 +3763,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>[A3220] WEST CROSS ROUTE (W10,W11,W12) (Hammersmith &amp; Fulham,Kensington &amp; Chelsea)</t>
+          <t>[A3220] BATTERSEA BRIDGE ROAD (SW11) (Kensington &amp; Chelsea,Wandsworth)</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -3765,7 +3773,7 @@
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.221082, 51.51375], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.169931, 51.478281], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T28" t="b">
@@ -3789,16 +3797,8 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y28" t="inlineStr">
-        <is>
-          <t>{'type': 'Polygon', 'coordinates': [[[-0.2268504991, 51.515214368], [-0.226816068, 51.5150759665], [-0.2266923055, 51.5149322348], [-0.2264944531, 51.5148255447], [-0.22624859, 51.514769959], [-0.2222289851, 51.5150082855], [-0.2221113839, 51.5148973036], [-0.2218935207, 51.5147814334], [-0.2217342167, 51.5146209077], [-0.2217165117, 51.5145590974], [-0.2219898415, 51.5142281809], [-0.2221301141, 51.5139454523], [-0.2221449065, 51.5138085631], [-0.2220721873, 51.5134910081], [-0.2205678856, 51.5111075751], [-0.2202148706, 51.5103339389], [-0.2198150378, 51.5091676116], [-0.219675534, 51.5090076612], [-0.2194415557, 51.5088941611], [-0.219086057, 51.5078415649], [-0.2185897904, 51.5066539009], [-0.2182414931, 51.5060381507], [-0.2173647255, 51.5048234777], [-0.2172272759, 51.504723302], [-0.2170491482, 51.5046523398], [-0.2168456828, 51.5046167021], [-0.2166344017, 51.5046194581], [-0.2163718851, 51.5046819683], [-0.2161676828, 51.5048024144], [-0.2160458612, 51.5049840778], [-0.2160517337, 51.5051593879], [-0.2162922472, 51.5055614647], [-0.2169077501, 51.5063788767], [-0.2174019457, 51.507321224], [-0.2186336527, 51.5107487541], [-0.2188885584, 51.5113469276], [-0.2192122199, 51.5118264977], [-0.2200716324, 51.5139055816], [-0.2201046988, 51.5140623912], [-0.2200137181, 51.5143839594], [-0.2195736429, 51.5148589248], [-0.2195083826, 51.515117759], [-0.2174597629, 51.5152667541], [-0.2164061948, 51.5154031442], [-0.2158660738, 51.5155028114], [-0.215089151, 51.5157160863], [-0.2119022877, 51.5168006338], [-0.2085686825, 51.5175740516], [-0.2081537913, 51.5176956104], [-0.2073044872, 51.5179999791], [-0.206542063, 51.5183931404], [-0.2059257385, 51.5187789312], [-0.2042932064, 51.5200279103], [-0.2035689067, 51.5204350978], [-0.2032427421, 51.5205820065], [-0.2025200333, 51.5208331967], [-0.2016527864, 51.5210280674], [-0.2011710714, 51.5210932856], [-0.2001367564, 51.5211473219], [-0.1993063778, 51.5210932442], [-0.1986305215, 51.5209980488], [-0.1977979222, 51.5207917816], [-0.1944017809, 51.5197558416], [-0.1936473833, 51.5195739804], [-0.1927795272, 51.5194060024], [-0.1912417461, 51.519189227], [-0.1900168103, 51.5191038861], [-0.1848656155, 51.5190371619], [-0.1845973629, 51.5190895], [-0.1843816324, 51.5192018967], [-0.1842421283, 51.5193785497], [-0.1842307399, 51.5195537531], [-0.1843099996, 51.5196992406], [-0.184437376, 51.519804493], [-0.1846082423, 51.519882146], [-0.1848427707, 51.5199290971], [-0.1899539586, 51.5200020012], [-0.1910275156, 51.5200785533], [-0.1917208959, 51.5201644808], [-0.192967492, 51.5203817851], [-0.1938615219, 51.5205891585], [-0.1971821776, 51.5216043926], [-0.1982276319, 51.5218612247], [-0.1990755076, 51.5219805605], [-0.2000396338, 51.5220444521], [-0.2012151975, 51.5220008809], [-0.2020360143, 51.5218950351], [-0.2030802769, 51.5216616773], [-0.2040030068, 51.5213458102], [-0.2044268186, 51.5211572666], [-0.2049988503, 51.5208578957], [-0.2056305823, 51.5204459626], [-0.207001595, 51.5193777412], [-0.2076748052, 51.5189613218], [-0.2081285965, 51.5187382039], [-0.2084824166, 51.5186038176], [-0.20911363, 51.5184067448], [-0.2124946693, 51.5176200575], [-0.2132845634, 51.5173738454], [-0.2157446367, 51.5165166288], [-0.2163624004, 51.5163475389], [-0.2176701507, 51.5161561474], [-0.2213144853, 51.5158933476], [-0.2215298893, 51.5159391065], [-0.2217236504, 51.51594327], [-0.2262646465, 51.5156547616], [-0.2264817636, 51.5156054962], [-0.2266844629, 51.5155002741], [-0.2268128844, 51.5153565877], [-0.2268504991, 51.515214368]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="Z28" t="inlineStr">
-        <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A40] WESTWAY (W10,W12)', 'closure': 'Open', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.22613,51.515213],[-0.224382,51.515322]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.22246,51.515445],[-0.221651,51.515496]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.224382,51.515322],[-0.22246,51.515445]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A40] WESTWAY (W10,W12)', 'closure': 'Closed', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.22613,51.515213],[-0.224382,51.515322]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.22246,51.515445],[-0.221651,51.515496]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.224382,51.515322],[-0.22246,51.515445]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3220] WEST CROSS ROUTE (W10,W11,W12)', 'closure': 'Open', 'directions': 'Southbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.221122,51.514298],[-0.221294,51.51505]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.221294,51.51505],[-0.221576,51.515198]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219205,51.509571],[-0.220102,51.511615]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219126,51.509298],[-0.219205,51.509571]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.220102,51.511615],[-0.221122,51.514298]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3220] WEST CROSS ROUTE (W10,W11,W12)', 'closure': 'Open', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.218945,51.509605],[-0.218851,51.509321]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.218851,51.509321],[-0.218825,51.509249]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.218825,51.509249],[-0.217898,51.50678]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.220227,51.51509],[-0.221294,51.51505]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.220227,51.51509],[-0.219897,51.511684]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.217581,51.506219],[-0.216755,51.505063]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.217898,51.50678],[-0.217581,51.506219]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219897,51.511684],[-0.218945,51.509605]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.221294,51.51505],[-0.221576,51.515198]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3220] WEST CROSS ROUTE (W10,W11,W12)', 'closure': 'Open', 'directions': 'Southbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.221122,51.514298],[-0.221294,51.51505]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.221294,51.51505],[-0.221576,51.515198]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219205,51.509571],[-0.220102,51.511615]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219126,51.509298],[-0.219205,51.509571]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.220102,51.511615],[-0.221122,51.514298]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A40] WESTWAY (W10,W11,W2,W9)', 'closure': 'Open', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.18876,51.519534],[-0.189999,51.519553]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.184942,51.519484],[-0.18876,51.519534]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.216796,51.515809],[-0.21755,51.515713]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.189999,51.519553],[-0.201091,51.521558]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.219906,51.515542],[-0.22164,51.515415]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.21372,51.516707],[-0.216796,51.515809]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.21755,51.515713],[-0.219906,51.515542]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.207202,51.518621],[-0.210223,51.517678]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.201091,51.521558],[-0.207202,51.518621]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.210223,51.517678],[-0.21372,51.516707]]', 'sourceSystemId': 0}], 'sourceSystemId': 182512, 'sourceSystemKey': 'TIMS'}]</t>
-        </is>
-      </c>
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>TIMS-205670</t>
+          <t>TIMS-204963</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205670</t>
+          <t>/Road/All/Disruption/TIMS-204963</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>[-0.138828,51.524968]</t>
+          <t>[-0.051059,51.497108]</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -3836,42 +3836,42 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Borough works</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>[A501] Euston Road (Eastbound) at the junction of [A400] Hampstead Road - Eastbound footway and carriageway restrictions during Euston Tower Development. Lane 1 of 3 will be closed. From 31/01 - 04/03 northbound lane 1 (of 2) is closed.</t>
+          <t xml:space="preserve">Surrey Quays Road (Both directions) between [A200] Lower Road and Deal Porters Way - Road closure due to UKPN works. </t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t>Use an alternative route. Delays are possible on diversion.</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-01-22T08:08:40Z</t>
+          <t>2025-01-22T09:32:28Z</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>['inner ring']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>2025-01-09T08:00:00Z</t>
+          <t>2025-01-06T08:00:00Z</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>2025-03-07T18:00:00Z</t>
+          <t>2025-01-27T23:59:00Z</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>2025-01-22T08:08:48Z</t>
+          <t>2025-01-22T09:32:28Z</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>[A501] EUSTON ROAD (NW1,WC1H) (Camden,Westminster)</t>
+          <t>SURREY QUAYS ROAD (SE16) (Southwark)</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -3891,7 +3891,7 @@
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.138828, 51.524968], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.051059, 51.497108], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T29" t="b">
@@ -3915,8 +3915,16 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y29" t="inlineStr"/>
-      <c r="Z29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>{'type': 'Polygon', 'coordinates': [[[-0.0532202117, 51.4963035624], [-0.0531101128, 51.4960739009], [-0.0528690697, 51.4959268849], [-0.0525472474, 51.4958644434], [-0.0521712196, 51.4959132037], [-0.0516174361, 51.4961298027], [-0.0503558083, 51.4967719877], [-0.0498691758, 51.496890246], [-0.0495415109, 51.4970175148], [-0.0493385719, 51.4971906357], [-0.0492507999, 51.4973265335], [-0.0492421467, 51.4974936739], [-0.0493156798, 51.4976328251], [-0.0495914138, 51.4978127893], [-0.0499783293, 51.4978734978], [-0.0502397027, 51.4978367444], [-0.050501731, 51.4977155507], [-0.0509786307, 51.4975883274], [-0.0516983202, 51.4972665459], [-0.0524610818, 51.4968615851], [-0.052981877, 51.4966470183], [-0.0531610554, 51.4964915146], [-0.0532202117, 51.4963035624]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+        </is>
+      </c>
+      <c r="Z29" t="inlineStr">
+        <is>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'SURREY QUAYS ROAD (SE16)', 'closure': 'Closed', 'directions': 'Both directions', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.0525,51.496313],[-0.052391,51.49636]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.049954,51.497424],[-0.050301,51.497284]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052391,51.49636],[-0.052173,51.496447]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052039,51.496494],[-0.050301,51.497284]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052173,51.496447],[-0.052039,51.496494]]', 'sourceSystemId': 0}], 'sourceSystemId': 204963, 'sourceSystemKey': 'TIMS'}]</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3926,17 +3934,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>TIMS-204885</t>
+          <t>TIMS-206055</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204885</t>
+          <t>/Road/All/Disruption/TIMS-206055</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>[-0.169931,51.478281]</t>
+          <t>[-0.052654,51.55242]</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -3954,42 +3962,42 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>TfL works</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>[A3220] Battersea Bridge Road (Both directions) at the junction of Parkgate Road - Lane closure in place to facilitate Urban Realm Works.</t>
+          <t xml:space="preserve">[A107] Lower Clapton Road (Both directions) at the junction of Powerscroft Road - Temporary traffic signals are in operation to facilitate UKPN works.   </t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t xml:space="preserve">Traffic is flowing well. </t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-01-22T08:53:58Z</t>
+          <t>2025-01-22T20:57:09Z</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>['western cross route']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>2025-01-20T07:00:00Z</t>
+          <t>2025-01-19T06:00:00Z</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>2025-05-22T06:00:00Z</t>
+          <t>2025-01-24T23:00:00Z</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>2025-01-22T08:53:58Z</t>
+          <t>2025-01-22T20:57:09Z</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3999,7 +4007,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>[A3220] BATTERSEA BRIDGE ROAD (SW11) (Kensington &amp; Chelsea,Wandsworth)</t>
+          <t>[A107] LOWER CLAPTON ROAD (E5,E8,E9) (Hackney)</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -4009,7 +4017,7 @@
       </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.169931, 51.478281], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.052654, 51.55242], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T30" t="b">
@@ -4044,17 +4052,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>TIMS-206121</t>
+          <t>TIMS-206054</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206121</t>
+          <t>/Road/All/Disruption/TIMS-206054</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[-0.219026,51.55979]</t>
+          <t>[-0.12737,51.509315]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -4077,17 +4085,17 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t xml:space="preserve">[A5] Cricklewood Broadway (All directions) at the junction of Mora Road - Temporary traffic signals are in operation to facilitate Thames Water works. </t>
+          <t>[A400] St Martins Place (All directions) at the junction of [A400] Charing Cross Road - Temporary signals in operation to facilitate Cadent Gas works.</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-01-22T08:26:09Z</t>
+          <t>2025-01-22T20:48:50Z</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -4097,7 +4105,7 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>2025-01-21T15:16:00Z</t>
+          <t>2025-01-19T17:45:00Z</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
@@ -4107,7 +4115,7 @@
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>2025-01-22T08:27:47Z</t>
+          <t>2025-01-22T20:48:50Z</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -4117,7 +4125,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>[A5] CRICKLEWOOD BROADWAY (NW2) (Barnet,Brent)</t>
+          <t>[A400] ST MARTINS PLACE (WC2N) (Westminster)</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -4127,7 +4135,7 @@
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.219026, 51.55979], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.12737, 51.509315], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T31" t="b">
@@ -4280,17 +4288,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>TIMS-205753</t>
+          <t>TIMS-206069</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205753</t>
+          <t>/Road/All/Disruption/TIMS-206069</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>[-0.077317,51.453151]</t>
+          <t>[-0.156729,51.49289]</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -4313,17 +4321,17 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t xml:space="preserve">[A2216] Lordship Lane (All directions) at the junction of Heber Road - Temporary traffic signals are in operation to facilitate Thames Water works. </t>
+          <t>[A3216] Sloane Square (Eastbound) at the junction of Sedding Street - Road is closed due to emergency Thames Water and Cadent Gas works</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t>Use an alternative route. There are no reported delays on diversion.</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-01-22T09:33:22Z</t>
+          <t>2025-01-22T20:49:07Z</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -4333,17 +4341,17 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>2025-01-18T10:00:00Z</t>
+          <t>2025-01-20T10:00:00Z</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>2025-01-28T18:00:00Z</t>
+          <t>2025-01-25T18:00:00Z</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>2025-01-22T09:33:32Z</t>
+          <t>2025-01-22T20:49:07Z</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -4353,7 +4361,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>[A2216] LORDSHIP LANE (SE22) (Southwark)</t>
+          <t>[A3216] SLOANE SQUARE (SW1W,SW1X,SW3) (Kensington &amp; Chelsea,Westminster)</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -4363,7 +4371,7 @@
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.077317, 51.453151], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.156729, 51.49289], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T33" t="b">
@@ -4387,8 +4395,16 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y33" t="inlineStr"/>
-      <c r="Z33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>{'type': 'Polygon', 'coordinates': [[[-0.1584777328, 51.4926860385], [-0.1584390066, 51.4925397983], [-0.1583261769, 51.4924093762], [-0.1581841856, 51.4923230989], [-0.1579722888, 51.4922562091], [-0.1576578673, 51.4922401505], [-0.1567956082, 51.4923397904], [-0.1558023405, 51.4927240695], [-0.1554594231, 51.4928949283], [-0.1552773642, 51.4931060012], [-0.1552950424, 51.4933454702], [-0.155432758, 51.4934983005], [-0.1556536853, 51.4936065998], [-0.1559241899, 51.4936538801], [-0.1562030893, 51.4936329433], [-0.1573164311, 51.4931897744], [-0.1579570413, 51.4931170608], [-0.1581784603, 51.4930499167], [-0.1583835504, 51.4929074402], [-0.1584777328, 51.4926860385]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+        </is>
+      </c>
+      <c r="Z33" t="inlineStr">
+        <is>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3216] SLOANE SQUARE (SW1W,SW1X,SW3)', 'closure': 'Closed', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.156313,51.493054],[-0.155979,51.493206]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157034,51.492764],[-0.15677,51.492877]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157758,51.492685],[-0.157034,51.492764]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.15677,51.492877],[-0.156313,51.493054]]', 'sourceSystemId': 0}], 'sourceSystemId': 206069, 'sourceSystemKey': 'TIMS'}]</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4398,17 +4414,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>TIMS-206055</t>
+          <t>TIMS-206121</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206055</t>
+          <t>/Road/All/Disruption/TIMS-206121</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[-0.052654,51.55242]</t>
+          <t>[-0.219026,51.55979]</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -4431,17 +4447,17 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t xml:space="preserve">[A107] Lower Clapton Road (Both directions) at the junction of Powerscroft Road - Temporary traffic signals are in operation to facilitate UKPN works.   </t>
+          <t xml:space="preserve">[A5] Cricklewood Broadway (All directions) at the junction of Mora Road - Temporary traffic signals are in operation to facilitate Thames Water works. </t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traffic is flowing well. </t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-01-22T18:30:19Z</t>
+          <t>2025-01-22T08:26:09Z</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -4451,17 +4467,17 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>2025-01-19T06:00:00Z</t>
+          <t>2025-01-21T15:16:00Z</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>2025-01-24T23:00:00Z</t>
+          <t>2025-01-24T17:00:00Z</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>2025-01-22T18:30:19Z</t>
+          <t>2025-01-22T08:27:47Z</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -4471,7 +4487,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>[A107] LOWER CLAPTON ROAD (E5,E8,E9) (Hackney)</t>
+          <t>[A5] CRICKLEWOOD BROADWAY (NW2) (Barnet,Brent)</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -4481,7 +4497,7 @@
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.052654, 51.55242], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.219026, 51.55979], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T34" t="b">
@@ -4516,17 +4532,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>TIMS-206069</t>
+          <t>TIMS-205753</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206069</t>
+          <t>/Road/All/Disruption/TIMS-205753</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>[-0.156729,51.49289]</t>
+          <t>[-0.077317,51.453151]</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -4549,17 +4565,17 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>[A3216] Sloane Square (Eastbound) at the junction of Sedding Street - Road is closed due to emergency Thames Water and Cadent Gas works</t>
+          <t xml:space="preserve">[A2216] Lordship Lane (All directions) at the junction of Heber Road - Temporary traffic signals are in operation to facilitate Thames Water works. </t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Use an alternative route. There are no reported delays on diversion.</t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-01-22T20:49:07Z</t>
+          <t>2025-01-22T09:33:22Z</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -4569,17 +4585,17 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>2025-01-20T10:00:00Z</t>
+          <t>2025-01-18T10:00:00Z</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>2025-01-25T18:00:00Z</t>
+          <t>2025-01-28T18:00:00Z</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>2025-01-22T20:49:07Z</t>
+          <t>2025-01-22T09:33:32Z</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -4589,7 +4605,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>[A3216] SLOANE SQUARE (SW1W,SW1X,SW3) (Kensington &amp; Chelsea,Westminster)</t>
+          <t>[A2216] LORDSHIP LANE (SE22) (Southwark)</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -4599,7 +4615,7 @@
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.156729, 51.49289], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.077317, 51.453151], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T35" t="b">
@@ -4623,16 +4639,8 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y35" t="inlineStr">
-        <is>
-          <t>{'type': 'Polygon', 'coordinates': [[[-0.1584777328, 51.4926860385], [-0.1584390066, 51.4925397983], [-0.1583261769, 51.4924093762], [-0.1581841856, 51.4923230989], [-0.1579722888, 51.4922562091], [-0.1576578673, 51.4922401505], [-0.1567956082, 51.4923397904], [-0.1558023405, 51.4927240695], [-0.1554594231, 51.4928949283], [-0.1552773642, 51.4931060012], [-0.1552950424, 51.4933454702], [-0.155432758, 51.4934983005], [-0.1556536853, 51.4936065998], [-0.1559241899, 51.4936538801], [-0.1562030893, 51.4936329433], [-0.1573164311, 51.4931897744], [-0.1579570413, 51.4931170608], [-0.1581784603, 51.4930499167], [-0.1583835504, 51.4929074402], [-0.1584777328, 51.4926860385]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="Z35" t="inlineStr">
-        <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3216] SLOANE SQUARE (SW1W,SW1X,SW3)', 'closure': 'Closed', 'directions': 'Eastbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.156313,51.493054],[-0.155979,51.493206]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157034,51.492764],[-0.15677,51.492877]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157758,51.492685],[-0.157034,51.492764]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.15677,51.492877],[-0.156313,51.493054]]', 'sourceSystemId': 0}], 'sourceSystemId': 206069, 'sourceSystemKey': 'TIMS'}]</t>
-        </is>
-      </c>
+      <c r="Y35" t="inlineStr"/>
+      <c r="Z35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4642,17 +4650,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>TIMS-204963</t>
+          <t>TIMS-205421</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204963</t>
+          <t>/Road/All/Disruption/TIMS-205421</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>[-0.051059,51.497108]</t>
+          <t>[-0.157309,51.491382]</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -4675,17 +4683,17 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Surrey Quays Road (Both directions) between [A200] Lower Road and Deal Porters Way - Road closure due to UKPN works. </t>
+          <t>[A3216] Lower Sloane Street (Northbound) between Sloane Gardens and [A3216] Sloane Square - Road closed due to Cadent Gas works.</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Use an alternative route. Delays are possible on diversion.</t>
+          <t xml:space="preserve">Use an alternative route. Delays are possible on diversion. </t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-01-22T09:32:28Z</t>
+          <t>2025-01-22T08:10:41Z</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -4695,17 +4703,17 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>2025-01-06T08:00:00Z</t>
+          <t>2025-01-07T08:00:00Z</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>2025-01-27T23:59:00Z</t>
+          <t>2025-02-07T23:59:00Z</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>2025-01-22T09:32:28Z</t>
+          <t>2025-01-22T08:10:50Z</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -4715,7 +4723,7 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>SURREY QUAYS ROAD (SE16) (Southwark)</t>
+          <t>[A3216] LOWER SLOANE STREET (SW1W) (Kensington &amp; Chelsea,Westminster)</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -4725,7 +4733,7 @@
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.051059, 51.497108], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.157309, 51.491382], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T36" t="b">
@@ -4751,12 +4759,12 @@
       </c>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>{'type': 'Polygon', 'coordinates': [[[-0.0532202117, 51.4963035624], [-0.0531101128, 51.4960739009], [-0.0528690697, 51.4959268849], [-0.0525472474, 51.4958644434], [-0.0521712196, 51.4959132037], [-0.0516174361, 51.4961298027], [-0.0503558083, 51.4967719877], [-0.0498691758, 51.496890246], [-0.0495415109, 51.4970175148], [-0.0493385719, 51.4971906357], [-0.0492507999, 51.4973265335], [-0.0492421467, 51.4974936739], [-0.0493156798, 51.4976328251], [-0.0495914138, 51.4978127893], [-0.0499783293, 51.4978734978], [-0.0502397027, 51.4978367444], [-0.050501731, 51.4977155507], [-0.0509786307, 51.4975883274], [-0.0516983202, 51.4972665459], [-0.0524610818, 51.4968615851], [-0.052981877, 51.4966470183], [-0.0531610554, 51.4964915146], [-0.0532202117, 51.4963035624]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Polygon', 'coordinates': [[[-0.1585161992, 51.4923536707], [-0.158444402, 51.492150888], [-0.1582249725, 51.491985707], [-0.1577718602, 51.4905380826], [-0.1575980485, 51.4904003359], [-0.1573530268, 51.4903145974], [-0.1570740974, 51.4902939198], [-0.1568037246, 51.4903414512], [-0.1566315522, 51.4904178771], [-0.1565023317, 51.4905222123], [-0.1564107106, 51.490755013], [-0.1568636923, 51.4923351459], [-0.1569470434, 51.4924763057], [-0.1571566938, 51.4926279809], [-0.157447094, 51.4927396166], [-0.1576643667, 51.4927884267], [-0.1578952185, 51.492791787], [-0.1581158996, 51.4927493517], [-0.1583355395, 51.4926444348], [-0.1584756066, 51.4924955697], [-0.1585161992, 51.4923536707]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'SURREY QUAYS ROAD (SE16)', 'closure': 'Closed', 'directions': 'Both directions', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.0525,51.496313],[-0.052391,51.49636]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.049954,51.497424],[-0.050301,51.497284]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052391,51.49636],[-0.052173,51.496447]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052039,51.496494],[-0.050301,51.497284]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.052173,51.496447],[-0.052039,51.496494]]', 'sourceSystemId': 0}], 'sourceSystemId': 204963, 'sourceSystemKey': 'TIMS'}]</t>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3216] LOWER SLOANE STREET (SW1W)', 'closure': 'Closed', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157571,51.492253],[-0.157796,51.492347]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157571,51.492253],[-0.15713,51.490742]]', 'sourceSystemId': 0}], 'sourceSystemId': 205421, 'sourceSystemKey': 'TIMS'}]</t>
         </is>
       </c>
     </row>
@@ -4768,17 +4776,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>TIMS-205421</t>
+          <t>TIMS-205742</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205421</t>
+          <t>/Road/All/Disruption/TIMS-205742</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[-0.157309,51.491382]</t>
+          <t>[-0.063863,51.473961]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -4796,52 +4804,52 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>TfL works</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>[A3216] Lower Sloane Street (Northbound) between Sloane Gardens and [A3216] Sloane Square - Road closed due to Cadent Gas works.</t>
+          <t>[A202] Peckham High Street (Southbound) between Consort Road and [A2215] Clayton Road - Southbound lane closures in operation to facilitate maintenance works.</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Use an alternative route. Delays are possible on diversion. </t>
+          <t>Some delays maybe experienced while this work takes place.</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-01-22T08:10:41Z</t>
+          <t>2025-01-22T20:07:37Z</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['a20']</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>2025-01-07T08:00:00Z</t>
+          <t>2025-01-22T20:00:00Z</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>2025-02-07T23:59:00Z</t>
+          <t>2025-01-23T06:00:00Z</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>2025-01-22T08:10:50Z</t>
+          <t>2025-01-22T20:07:39Z</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>[A3216] LOWER SLOANE STREET (SW1W) (Kensington &amp; Chelsea,Westminster)</t>
+          <t>[A202] PECKHAM HIGH STREET (SE15) (Southwark)</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -4851,7 +4859,7 @@
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.157309, 51.491382], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.063863, 51.473961], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T37" t="b">
@@ -4875,16 +4883,8 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y37" t="inlineStr">
-        <is>
-          <t>{'type': 'Polygon', 'coordinates': [[[-0.1585161992, 51.4923536707], [-0.158444402, 51.492150888], [-0.1582249725, 51.491985707], [-0.1577718602, 51.4905380826], [-0.1575980485, 51.4904003359], [-0.1573530268, 51.4903145974], [-0.1570740974, 51.4902939198], [-0.1568037246, 51.4903414512], [-0.1566315522, 51.4904178771], [-0.1565023317, 51.4905222123], [-0.1564107106, 51.490755013], [-0.1568636923, 51.4923351459], [-0.1569470434, 51.4924763057], [-0.1571566938, 51.4926279809], [-0.157447094, 51.4927396166], [-0.1576643667, 51.4927884267], [-0.1578952185, 51.492791787], [-0.1581158996, 51.4927493517], [-0.1583355395, 51.4926444348], [-0.1584756066, 51.4924955697], [-0.1585161992, 51.4923536707]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="Z37" t="inlineStr">
-        <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A3216] LOWER SLOANE STREET (SW1W)', 'closure': 'Closed', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157571,51.492253],[-0.157796,51.492347]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.157571,51.492253],[-0.15713,51.490742]]', 'sourceSystemId': 0}], 'sourceSystemId': 205421, 'sourceSystemKey': 'TIMS'}]</t>
-        </is>
-      </c>
+      <c r="Y37" t="inlineStr"/>
+      <c r="Z37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4894,17 +4894,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>TIMS-206054</t>
+          <t>TIMS-203041</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206054</t>
+          <t>/Road/All/Disruption/TIMS-203041</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>[-0.12737,51.509315]</t>
+          <t>[-0.010106,51.461524]</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -4922,52 +4922,52 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>Borough works</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>[A400] St Martins Place (All directions) at the junction of [A400] Charing Cross Road - Temporary signals in operation to facilitate Cadent Gas works.</t>
+          <t>Lewisham High Street (Northbound) at the junction of Lewis Grove - Road closure northbound between Lewisham High Street and Lee Bridge to facilitate works.</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Traffic is flowing well.</t>
+          <t>Use an alternative route. Delays are possible on diversion.</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-01-22T20:48:50Z</t>
+          <t>2025-01-22T09:31:03Z</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['a20', 'a21']</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>2025-01-19T17:45:00Z</t>
+          <t>2024-08-03T07:00:00Z</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>2025-01-24T17:00:00Z</t>
+          <t>2025-03-31T17:00:00Z</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>2025-01-22T20:48:50Z</t>
+          <t>2025-01-22T09:31:14Z</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>[A400] ST MARTINS PLACE (WC2N) (Westminster)</t>
+          <t>LEWISHAM HIGH STREET (SE13) (Lewisham)</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -4977,7 +4977,7 @@
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.12737, 51.509315], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.010106, 51.461524], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T38" t="b">
@@ -5001,8 +5001,16 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y38" t="inlineStr"/>
-      <c r="Z38" t="inlineStr"/>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>{'type': 'Polygon', 'coordinates': [[[-0.012734878, 51.4593126239], [-0.0126900506, 51.4591409421], [-0.0125806121, 51.4590193676], [-0.0124167755, 51.4589246095], [-0.0122143225, 51.4588657953], [-0.011992754, 51.4588485902], [-0.0117734125, 51.4588746513], [-0.0115774255, 51.4589414685], [-0.0113907291, 51.4590667721], [-0.0111057165, 51.4594449735], [-0.010635101, 51.459946833], [-0.0099789336, 51.4607894854], [-0.009678438, 51.4610565384], [-0.009604918, 51.4611951152], [-0.0093358373, 51.4612878686], [-0.0091500677, 51.4614469781], [-0.0086289053, 51.462360547], [-0.008690566, 51.4625971575], [-0.0089381945, 51.4627803029], [-0.0091964122, 51.4628490915], [-0.0094771174, 51.4628509183], [-0.0097375735, 51.4627855052], [-0.009938127, 51.4626628111], [-0.0105206374, 51.4616962362], [-0.0108456493, 51.4615692905], [-0.0112195757, 51.4612465742], [-0.0120015704, 51.4602565133], [-0.0124604446, 51.4597553773], [-0.0126555264, 51.4596022293], [-0.0127163805, 51.4594883868], [-0.012734878, 51.4593126239]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+        </is>
+      </c>
+      <c r="Z38" t="inlineStr">
+        <is>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'LEWIS GROVE (SE13)', 'closure': 'Closed', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.009344,51.462409],[-0.00981,51.461626]]', 'sourceSystemId': 0}], 'sourceSystemId': 203041, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A21] LEWISHAM HIGH STREET (SE13)', 'closure': 'Closed', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.012008,51.459406],[-0.012016,51.459298]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010315,51.461266],[-0.010405,51.461195]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010405,51.461195],[-0.010736,51.46085]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.011773,51.459625],[-0.012016,51.459298]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.011773,51.459625],[-0.010951,51.460548]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010951,51.460548],[-0.010736,51.46085]]', 'sourceSystemId': 0}], 'sourceSystemId': 203041, 'sourceSystemKey': 'TIMS'}]</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5012,17 +5020,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>TIMS-203041</t>
+          <t>TIMS-205898</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-203041</t>
+          <t>/Road/All/Disruption/TIMS-205898</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>[-0.010106,51.461524]</t>
+          <t>[0.000174,51.458561]</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -5040,42 +5048,42 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Borough works</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Lewisham High Street (Northbound) at the junction of Lewis Grove - Road closure northbound between Lewisham High Street and Lee Bridge to facilitate works.</t>
+          <t>[A20] Lee High Road (Both directions) at the junction of Glenton Road - Two-way temporary traffic signals in place to facilitate SGN works.</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Use an alternative route. Delays are possible on diversion.</t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-01-22T09:31:03Z</t>
+          <t>2025-01-22T09:26:00Z</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>['a20', 'a21']</t>
+          <t>['a20']</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>2024-08-03T07:00:00Z</t>
+          <t>2025-01-15T12:05:00Z</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>2025-03-31T17:00:00Z</t>
+          <t>2025-01-23T23:59:00Z</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>2025-01-22T09:31:14Z</t>
+          <t>2025-01-22T09:26:00Z</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -5085,7 +5093,7 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>LEWISHAM HIGH STREET (SE13) (Lewisham)</t>
+          <t>[A20] LEE HIGH ROAD (SE12,SE13,SE3) (Lewisham)</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -5095,7 +5103,7 @@
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.010106, 51.461524], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [0.000174, 51.458561], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T39" t="b">
@@ -5119,16 +5127,8 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="Y39" t="inlineStr">
-        <is>
-          <t>{'type': 'Polygon', 'coordinates': [[[-0.012734878, 51.4593126239], [-0.0126900506, 51.4591409421], [-0.0125806121, 51.4590193676], [-0.0124167755, 51.4589246095], [-0.0122143225, 51.4588657953], [-0.011992754, 51.4588485902], [-0.0117734125, 51.4588746513], [-0.0115774255, 51.4589414685], [-0.0113907291, 51.4590667721], [-0.0111057165, 51.4594449735], [-0.010635101, 51.459946833], [-0.0099789336, 51.4607894854], [-0.009678438, 51.4610565384], [-0.009604918, 51.4611951152], [-0.0093358373, 51.4612878686], [-0.0091500677, 51.4614469781], [-0.0086289053, 51.462360547], [-0.008690566, 51.4625971575], [-0.0089381945, 51.4627803029], [-0.0091964122, 51.4628490915], [-0.0094771174, 51.4628509183], [-0.0097375735, 51.4627855052], [-0.009938127, 51.4626628111], [-0.0105206374, 51.4616962362], [-0.0108456493, 51.4615692905], [-0.0112195757, 51.4612465742], [-0.0120015704, 51.4602565133], [-0.0124604446, 51.4597553773], [-0.0126555264, 51.4596022293], [-0.0127163805, 51.4594883868], [-0.012734878, 51.4593126239]]], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="Z39" t="inlineStr">
-        <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': 'LEWIS GROVE (SE13)', 'closure': 'Closed', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.009344,51.462409],[-0.00981,51.461626]]', 'sourceSystemId': 0}], 'sourceSystemId': 203041, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A21] LEWISHAM HIGH STREET (SE13)', 'closure': 'Closed', 'directions': 'Northbound', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.012008,51.459406],[-0.012016,51.459298]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010315,51.461266],[-0.010405,51.461195]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010405,51.461195],[-0.010736,51.46085]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.011773,51.459625],[-0.012016,51.459298]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.011773,51.459625],[-0.010951,51.460548]]', 'sourceSystemId': 0}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '0', 'lineString': '[[-0.010951,51.460548],[-0.010736,51.46085]]', 'sourceSystemId': 0}], 'sourceSystemId': 203041, 'sourceSystemKey': 'TIMS'}]</t>
-        </is>
-      </c>
+      <c r="Y39" t="inlineStr"/>
+      <c r="Z39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5138,17 +5138,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>TIMS-205742</t>
+          <t>TIMS-206068</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205742</t>
+          <t>/Road/All/Disruption/TIMS-206068</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[-0.063863,51.473961]</t>
+          <t>[-0.193207,51.457005]</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -5166,42 +5166,42 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>TfL works</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>[A202] Peckham High Street (Southbound) between Consort Road and [A2215] Clayton Road - Southbound lane closures in operation to facilitate maintenance works.</t>
+          <t>[A3] Wandsworth High Street (Westbound) at the junction of [A217] Ram Street - Lanes two and three (of three) is blocked due to emergency Thames Water works.</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Some delays maybe experienced while this work takes place.</t>
+          <t>Traffic is flowing well past the works.</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-01-22T20:07:37Z</t>
+          <t>2025-01-22T19:11:19Z</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>['a20']</t>
+          <t>['a205']</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>2025-01-22T20:00:00Z</t>
+          <t>2025-01-20T10:05:00Z</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>2025-01-23T06:00:00Z</t>
+          <t>2025-02-04T18:00:00Z</t>
         </is>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>2025-01-22T20:07:39Z</t>
+          <t>2025-01-22T19:11:19Z</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -5211,7 +5211,7 @@
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>[A202] PECKHAM HIGH STREET (SE15) (Southwark)</t>
+          <t>[A3] WANDSWORTH HIGH STREET (SW18) (Wandsworth)</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -5221,7 +5221,7 @@
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.063863, 51.473961], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.193207, 51.457005], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T40" t="b">
@@ -5256,17 +5256,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>TIMS-205898</t>
+          <t>TIMS-205100</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205898</t>
+          <t>/Road/All/Disruption/TIMS-205100</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>[0.000174,51.458561]</t>
+          <t>[-0.105897,51.441005]</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -5289,37 +5289,37 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>[A20] Lee High Road (Both directions) at the junction of Glenton Road - Two-way temporary traffic signals in place to facilitate SGN works.</t>
+          <t>[A205] Thurlow Park Road (Eastbound) at the junction of [A215] Norwood Road - Lane one closure eastbound to facilitate Thames Water works.</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t>Traffic is flowing well past the works.</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-01-22T09:26:00Z</t>
+          <t>2025-01-22T19:09:16Z</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>['a20']</t>
+          <t>['a205']</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>2025-01-15T12:05:00Z</t>
+          <t>2025-01-21T08:00:00Z</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>2025-01-23T23:59:00Z</t>
+          <t>2025-01-29T17:00:00Z</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>2025-01-22T09:26:00Z</t>
+          <t>2025-01-22T19:11:09Z</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>[A20] LEE HIGH ROAD (SE12,SE13,SE3) (Lewisham)</t>
+          <t>[A205] THURLOW PARK ROAD (SE21,SE24,SE27) (Lambeth)</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -5339,7 +5339,7 @@
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [0.000174, 51.458561], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.105897, 51.441005], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T41" t="b">
@@ -5374,17 +5374,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>TIMS-206068</t>
+          <t>TIMS-205629</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206068</t>
+          <t>/Road/All/Disruption/TIMS-205629</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>[-0.193207,51.457005]</t>
+          <t>[-0.253857,51.437053]</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -5407,37 +5407,37 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>[A3] Wandsworth High Street (Westbound) at the junction of [A217] Ram Street - Lanes two and three (of three) is blocked due to emergency Thames Water works.</t>
+          <t>[A3] Roehampton Vale (Westbound) at the junction of [A3] Kingston Vale - Thames Water works. The slip road from westbound A3 Roehampton Vale into A308 Kingston Vale is closed.</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Traffic is flowing well past the works.</t>
+          <t>Use an alternative route. Delays are possible.</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-01-22T19:11:19Z</t>
+          <t>2025-01-22T09:41:10Z</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>['a205']</t>
+          <t>['a3']</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>2025-01-20T10:05:00Z</t>
+          <t>2025-01-08T16:45:00Z</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>2025-02-04T18:00:00Z</t>
+          <t>2025-01-29T17:00:00Z</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>2025-01-22T19:11:19Z</t>
+          <t>2025-01-22T09:41:22Z</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -5447,7 +5447,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>[A3] WANDSWORTH HIGH STREET (SW18) (Wandsworth)</t>
+          <t>[A3] ROEHAMPTON VALE (SW15) (Kingston upon Thames,Wandsworth)</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -5457,7 +5457,7 @@
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.193207, 51.457005], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.253857, 51.437053], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T42" t="b">
@@ -5492,17 +5492,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>TIMS-205100</t>
+          <t>TIMS-206145</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205100</t>
+          <t>/Road/All/Disruption/TIMS-206145</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[-0.105897,51.441005]</t>
+          <t>[-0.198331,51.491627]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -5525,37 +5525,37 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>[A205] Thurlow Park Road (Eastbound) at the junction of [A215] Norwood Road - Lane one closure eastbound to facilitate Thames Water works.</t>
+          <t>[A3220] Warwick Road (Northbound) at the junction of Nevern Square - Lane closure in place to facilitate UKPN works.</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Traffic is flowing well past the works.</t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-01-22T19:09:16Z</t>
+          <t>2025-01-22T20:48:41Z</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>['a205']</t>
+          <t>['a4', 'western cross route']</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>2025-01-21T08:00:00Z</t>
+          <t>2025-01-22T08:00:00Z</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>2025-01-29T17:00:00Z</t>
+          <t>2025-02-05T18:00:00Z</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>2025-01-22T19:11:09Z</t>
+          <t>2025-01-22T20:48:41Z</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -5565,7 +5565,7 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>[A205] THURLOW PARK ROAD (SE21,SE24,SE27) (Lambeth)</t>
+          <t>[A3220] WARWICK ROAD (SW10,SW5,W14,W8) (Kensington &amp; Chelsea)</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -5575,7 +5575,7 @@
       </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.105897, 51.441005], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.198331, 51.491627], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T43" t="b">
@@ -5610,17 +5610,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>TIMS-205629</t>
+          <t>TIMS-205539</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205629</t>
+          <t>/Road/All/Disruption/TIMS-205539</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>[-0.253857,51.437053]</t>
+          <t>[-0.167464,51.518121]</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -5643,37 +5643,37 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>[A3] Roehampton Vale (Westbound) at the junction of [A3] Kingston Vale - Thames Water works. The slip road from westbound A3 Roehampton Vale into A308 Kingston Vale is closed.</t>
+          <t>[A5] Edgware Road (Southbound) at the junction of [A501] Old Marylebone Road - Lane one (of two ) closure due to utility works</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Use an alternative route. Delays are possible.</t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-01-22T09:41:10Z</t>
+          <t>2025-01-22T20:05:46Z</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>['a3']</t>
+          <t>['a40', 'a41', 'inner ring']</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>2025-01-08T16:45:00Z</t>
+          <t>2025-01-22T20:01:00Z</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>2025-01-29T17:00:00Z</t>
+          <t>2025-01-23T06:00:00Z</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>2025-01-22T09:41:22Z</t>
+          <t>2025-01-22T20:05:48Z</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -5683,7 +5683,7 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>[A3] ROEHAMPTON VALE (SW15) (Kingston upon Thames,Wandsworth)</t>
+          <t>[A5] EDGWARE ROAD (NW1,NW8,W1H,W2) (Westminster)</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -5693,7 +5693,7 @@
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.253857, 51.437053], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.167464, 51.518121], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T44" t="b">
@@ -5728,17 +5728,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TIMS-206145</t>
+          <t>TIMS-205970</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-206145</t>
+          <t>/Road/All/Disruption/TIMS-205970</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>[-0.198331,51.491627]</t>
+          <t>[-0.280535,51.47514]</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -5761,37 +5761,37 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>[A3220] Warwick Road (Northbound) at the junction of Nevern Square - Lane closure in place to facilitate UKPN works.</t>
+          <t>[A205] Mortlake Road (Both directions) at the junction of High Park Road - Road is closed in both directions to allow for essential road maintenance to be carried out by Thames Water</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Traffic is flowing well.</t>
+          <t>Use an alternative route. Delays are possible on diversion.</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-01-22T20:48:41Z</t>
+          <t>2025-01-22T09:39:37Z</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>['a4', 'western cross route']</t>
+          <t>['a406']</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>2025-01-22T08:00:00Z</t>
+          <t>2025-01-16T17:55:00Z</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>2025-02-05T18:00:00Z</t>
+          <t>2025-01-22T23:59:00Z</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>2025-01-22T20:48:41Z</t>
+          <t>2025-01-22T09:39:48Z</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -5801,7 +5801,7 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>[A3220] WARWICK ROAD (SW10,SW5,W14,W8) (Kensington &amp; Chelsea)</t>
+          <t>[A205] MORTLAKE ROAD (SW14,TW9) (Richmond upon Thames)</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -5811,7 +5811,7 @@
       </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.198331, 51.491627], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.280535, 51.47514], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T45" t="b">
@@ -5836,7 +5836,11 @@
         </is>
       </c>
       <c r="Y45" t="inlineStr"/>
-      <c r="Z45" t="inlineStr"/>
+      <c r="Z45" t="inlineStr">
+        <is>
+          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A205] MORTLAKE ROAD (TW9)', 'closure': 'Closed', 'directions': 'Both directions', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206507009', 'lineString': '[[-0.279734,51.474789],[-0.279608,51.474739]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206507010', 'lineString': '[[-0.279608,51.474739],[-0.279444,51.474692]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206509263', 'lineString': '[[-0.279792,51.474818],[-0.279734,51.474789]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}], 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}]</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5846,17 +5850,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TIMS-205539</t>
+          <t>TIMS-204896</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205539</t>
+          <t>/Road/All/Disruption/TIMS-204896</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[-0.167464,51.518121]</t>
+          <t>[-0.174162,51.53443]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -5879,7 +5883,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>[A5] Edgware Road (Southbound) at the junction of [A501] Old Marylebone Road - Lane one (of two ) closure due to utility works</t>
+          <t>Utility Works - Thames Water - [A41] Finchley Road (Both directions) at the junction of [A41] Wellington Road - Side road closures will be implemented with local diversions from the 6th of January to 3rd February to allow for water works by Thames Water.</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -5889,27 +5893,27 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-01-22T20:05:46Z</t>
+          <t>2025-01-22T20:33:47Z</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>['a40', 'a41', 'inner ring']</t>
+          <t>['a41']</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>2025-01-22T20:01:00Z</t>
+          <t>2025-01-12T08:00:00Z</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>2025-01-23T06:00:00Z</t>
+          <t>2025-01-12T18:00:00Z</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>2025-01-22T20:05:48Z</t>
+          <t>2025-01-22T20:33:47Z</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -5919,7 +5923,7 @@
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>[A5] EDGWARE ROAD (NW1,NW8,W1H,W2) (Westminster)</t>
+          <t>[A41] FINCHLEY ROAD (NW8) (Camden,Westminster)</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
@@ -5929,7 +5933,7 @@
       </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.167464, 51.518121], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.174162, 51.53443], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T46" t="b">
@@ -5964,17 +5968,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>TIMS-205970</t>
+          <t>TIMS-205973</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205970</t>
+          <t>/Road/All/Disruption/TIMS-205973</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>[-0.280535,51.47514]</t>
+          <t>[-0.084093,51.513343]</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -5992,42 +5996,42 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>TfL works</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>[A205] Mortlake Road (Both directions) at the junction of High Park Road - Road is closed in both directions to allow for essential road maintenance to be carried out by Thames Water</t>
+          <t>[A10] Gracechurch Street (Both directions) at the junction of Leadenhall Street - Lane restrictions to facilitate collaborative works.</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Use an alternative route. Delays are possible on diversion.</t>
+          <t xml:space="preserve">There are no reported delays. </t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-01-22T09:39:37Z</t>
+          <t>2025-01-22T20:48:58Z</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>['a406']</t>
+          <t>['bishopsgate cross route']</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>2025-01-16T17:55:00Z</t>
+          <t>2025-01-20T08:00:00Z</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>2025-01-22T23:59:00Z</t>
+          <t>2025-01-31T17:00:00Z</t>
         </is>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>2025-01-22T09:39:48Z</t>
+          <t>2025-01-22T20:48:58Z</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -6037,7 +6041,7 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>[A205] MORTLAKE ROAD (SW14,TW9) (Richmond upon Thames)</t>
+          <t>[A10] GRACECHURCH STREET (EC3V,EC4N,EC4R) (City of London)</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
@@ -6047,7 +6051,7 @@
       </c>
       <c r="S47" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.280535, 51.47514], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.084093, 51.513343], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T47" t="b">
@@ -6072,11 +6076,7 @@
         </is>
       </c>
       <c r="Y47" t="inlineStr"/>
-      <c r="Z47" t="inlineStr">
-        <is>
-          <t>[{'$type': 'Tfl.Api.Presentation.Entities.Street, Tfl.Api.Presentation.Entities', 'name': '[A205] MORTLAKE ROAD (TW9)', 'closure': 'Closed', 'directions': 'Both directions', 'segments': [{'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206507009', 'lineString': '[[-0.279734,51.474789],[-0.279608,51.474739]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206507010', 'lineString': '[[-0.279608,51.474739],[-0.279444,51.474692]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}, {'$type': 'Tfl.Api.Presentation.Entities.StreetSegment, Tfl.Api.Presentation.Entities', 'toid': '5000005206509263', 'lineString': '[[-0.279792,51.474818],[-0.279734,51.474789]]', 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}], 'sourceSystemId': 205970, 'sourceSystemKey': 'TIMS'}]</t>
-        </is>
-      </c>
+      <c r="Z47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6086,17 +6086,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>TIMS-204896</t>
+          <t>TIMS-204461</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204896</t>
+          <t>/Road/All/Disruption/TIMS-204461</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>[-0.174162,51.53443]</t>
+          <t>[-0.122625,51.494512]</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -6114,42 +6114,42 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>TfL works</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Utility Works - Thames Water - [A41] Finchley Road (Both directions) at the junction of [A41] Wellington Road - Side road closures will be implemented with local diversions from the 6th of January to 3rd February to allow for water works by Thames Water.</t>
+          <t xml:space="preserve">[A3203] Lambeth Bridge (Both directions) between [A3212] Millbank and [A3036] A 3036 - Various restrictions during junction improvement works at either side of Lambeth Bridge. Currently restrictions are in place on all approaches and inner ring of Lambeth Roundabout. From 30 January 21:30 until 07 February 05:00, there will be nightly road closures of Lambeth Bridge, Lambeth Palace Road, Lambeth Road &amp; Albert Embankment, with diversions in place via Westminster and Vauxhall Bridges. </t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Traffic is flowing well.</t>
+          <t xml:space="preserve">Delays are possible. </t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-01-22T20:33:47Z</t>
+          <t>2025-01-22T08:05:25Z</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>['a41']</t>
+          <t>['southern river route']</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>2025-01-12T08:00:00Z</t>
+          <t>2024-08-31T23:01:00Z</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>2025-01-12T18:00:00Z</t>
+          <t>2025-05-08T16:00:00Z</t>
         </is>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>2025-01-22T20:33:47Z</t>
+          <t>2025-01-22T08:05:34Z</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -6159,7 +6159,7 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>[A41] FINCHLEY ROAD (NW8) (Camden,Westminster)</t>
+          <t>[A3203] LAMBETH BRIDGE (SE1,SW1P) (Lambeth,Westminster)</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
@@ -6169,7 +6169,7 @@
       </c>
       <c r="S48" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.174162, 51.53443], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.122625, 51.494512], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T48" t="b">
@@ -6204,17 +6204,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>TIMS-205973</t>
+          <t>TIMS-205242</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205973</t>
+          <t>/Road/All/Disruption/TIMS-205242</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[-0.084093,51.513343]</t>
+          <t>[-0.077022,51.502078]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -6232,27 +6232,27 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>TfL works</t>
+          <t>Utility works</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>[A10] Gracechurch Street (Both directions) at the junction of Leadenhall Street - Lane restrictions to facilitate collaborative works.</t>
+          <t>[A200] Tooley Street (Both directions) at the junction of Boss Street - Lane restrictions in place to facilitate Southern Gas connection works.</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t xml:space="preserve">There are no reported delays. </t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-01-22T20:48:58Z</t>
+          <t>2025-01-22T07:52:18Z</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>['bishopsgate cross route']</t>
+          <t>['southern river route']</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
@@ -6262,12 +6262,12 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>2025-01-31T17:00:00Z</t>
+          <t>2025-01-24T18:00:00Z</t>
         </is>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>2025-01-22T20:48:58Z</t>
+          <t>2025-01-22T07:52:45Z</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -6277,7 +6277,7 @@
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>[A10] GRACECHURCH STREET (EC3V,EC4N,EC4R) (City of London)</t>
+          <t>[A200] TOOLEY STREET (SE1) (Southwark)</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -6287,7 +6287,7 @@
       </c>
       <c r="S49" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.084093, 51.513343], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.077022, 51.502078], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T49" t="b">
@@ -6322,17 +6322,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>TIMS-204461</t>
+          <t>TIMS-205243</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-204461</t>
+          <t>/Road/All/Disruption/TIMS-205243</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>[-0.122625,51.494512]</t>
+          <t>[-0.100283,51.493373]</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -6350,42 +6350,42 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>TfL works</t>
+          <t>Construction activity</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t xml:space="preserve">[A3203] Lambeth Bridge (Both directions) between [A3212] Millbank and [A3036] A 3036 - Various restrictions during junction improvement works at either side of Lambeth Bridge. Currently restrictions are in place on all approaches and inner ring of Lambeth Roundabout. From 30 January 21:30 until 07 February 05:00, there will be nightly road closures of Lambeth Bridge, Lambeth Palace Road, Lambeth Road &amp; Albert Embankment, with diversions in place via Westminster and Vauxhall Bridges. </t>
+          <t>[A215] Walworth Road (Southbound) at the junction of [A3] Newington Butts - Lane restriction contained to southbound Walworth Road to facilitate scaffolding works.</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delays are possible. </t>
+          <t>Delays are possible.</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-01-22T08:05:25Z</t>
+          <t>2025-01-22T08:12:06Z</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>['southern river route']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>2024-08-31T23:01:00Z</t>
+          <t>2025-01-13T08:00:00Z</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>2025-05-08T16:00:00Z</t>
+          <t>2025-10-03T22:59:00Z</t>
         </is>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>2025-01-22T08:05:34Z</t>
+          <t>2025-01-22T08:17:28Z</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -6395,7 +6395,7 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>[A3203] LAMBETH BRIDGE (SE1,SW1P) (Lambeth,Westminster)</t>
+          <t>[A215] WALWORTH ROAD (SE1,SE17) (Southwark)</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -6405,7 +6405,7 @@
       </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.122625, 51.494512], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.100283, 51.493373], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T50" t="b">
@@ -6440,17 +6440,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>TIMS-205242</t>
+          <t>TIMS-206136</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205242</t>
+          <t>/Road/All/Disruption/TIMS-206136</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>[-0.077022,51.502078]</t>
+          <t>[-0.170834,51.51835]</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -6468,12 +6468,12 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Utility works</t>
+          <t>Borough works</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>[A200] Tooley Street (Both directions) at the junction of Boss Street - Lane restrictions in place to facilitate Southern Gas connection works.</t>
+          <t>[A4205] Praed Street (Both directions) at the junction of Sale Place - Road works are being carried out at this location under temporary signals.</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -6483,27 +6483,27 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2025-01-22T07:52:18Z</t>
+          <t>2025-01-22T07:06:04Z</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>['southern river route']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>2025-01-20T08:00:00Z</t>
+          <t>2025-01-22T00:04:00Z</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>2025-01-24T18:00:00Z</t>
+          <t>2025-01-27T23:59:00Z</t>
         </is>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>2025-01-22T07:52:45Z</t>
+          <t>2025-01-22T07:06:38Z</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -6513,7 +6513,7 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>[A200] TOOLEY STREET (SE1) (Southwark)</t>
+          <t>[A4205] PRAED STREET (W2) (Westminster)</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
@@ -6523,7 +6523,7 @@
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.077022, 51.502078], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.170834, 51.51835], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T51" t="b">
@@ -6558,17 +6558,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>TIMS-205916</t>
+          <t>TIMS-205512</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205916</t>
+          <t>/Road/All/Disruption/TIMS-205512</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>[-0.343052,51.542371]</t>
+          <t>[-0.106039,51.556345]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -6581,27 +6581,27 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Works</t>
+          <t>Planned events</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Borough works</t>
+          <t>Sporting</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>[A4127] Greenford Road (Both directions) at the junction of Rockware Avenue - Temporary traffic signals in place to facilitate roadworks</t>
+          <t>Drayton Park (All approaches) at the junction of Aubert Park - Arsenal v Dynamo Zagreb Football Match.</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Traffic is flowing well.</t>
+          <t xml:space="preserve">Delays possible. </t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2025-01-22T20:34:13Z</t>
+          <t>2025-01-22T20:34:23Z</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -6611,17 +6611,17 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>2025-01-20T08:00:00Z</t>
+          <t>2025-01-22T19:00:00Z</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>2025-01-27T06:00:00Z</t>
+          <t>2025-01-22T22:30:00Z</t>
         </is>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>2025-01-22T20:34:13Z</t>
+          <t>2025-01-22T20:34:23Z</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -6631,7 +6631,7 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>[A4127] GREENFORD ROAD (UB5,UB6) (Ealing)</t>
+          <t>DRAYTON PARK (N5,N7) (Islington)</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -6641,7 +6641,7 @@
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.343052, 51.542371], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.106039, 51.556345], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T52" t="b">
@@ -6676,17 +6676,17 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>TIMS-205243</t>
+          <t>TIMS-205916</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>/Road/All/Disruption/TIMS-205243</t>
+          <t>/Road/All/Disruption/TIMS-205916</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>[-0.100283,51.493373]</t>
+          <t>[-0.343052,51.542371]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -6704,22 +6704,22 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Construction activity</t>
+          <t>Borough works</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>[A215] Walworth Road (Southbound) at the junction of [A3] Newington Butts - Lane restriction contained to southbound Walworth Road to facilitate scaffolding works.</t>
+          <t>[A4127] Greenford Road (Both directions) at the junction of Rockware Avenue - Temporary traffic signals in place to facilitate roadworks</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Delays are possible.</t>
+          <t>Traffic is flowing well.</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>2025-01-22T08:12:06Z</t>
+          <t>2025-01-22T20:34:13Z</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -6729,17 +6729,17 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>2025-01-13T08:00:00Z</t>
+          <t>2025-01-20T08:00:00Z</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>2025-10-03T22:59:00Z</t>
+          <t>2025-01-27T06:00:00Z</t>
         </is>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>2025-01-22T08:17:28Z</t>
+          <t>2025-01-22T20:34:13Z</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -6749,7 +6749,7 @@
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>[A215] WALWORTH ROAD (SE1,SE17) (Southwark)</t>
+          <t>[A4127] GREENFORD ROAD (UB5,UB6) (Ealing)</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -6759,7 +6759,7 @@
       </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>{'type': 'Point', 'coordinates': [-0.100283, 51.493373], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
+          <t>{'type': 'Point', 'coordinates': [-0.343052, 51.542371], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
         </is>
       </c>
       <c r="T53" t="b">
@@ -6785,242 +6785,6 @@
       </c>
       <c r="Y53" t="inlineStr"/>
       <c r="Z53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>Tfl.Api.Presentation.Entities.RoadDisruption, Tfl.Api.Presentation.Entities</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>TIMS-206136</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>/Road/All/Disruption/TIMS-206136</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>[-0.170834,51.51835]</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>Minimal</t>
-        </is>
-      </c>
-      <c r="F54" t="n">
-        <v>53</v>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Works</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Borough works</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>[A4205] Praed Street (Both directions) at the junction of Sale Place - Road works are being carried out at this location under temporary signals.</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>Delays are possible.</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>2025-01-22T07:06:04Z</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>2025-01-22T00:04:00Z</t>
-        </is>
-      </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>2025-01-27T23:59:00Z</t>
-        </is>
-      </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>2025-01-22T07:06:38Z</t>
-        </is>
-      </c>
-      <c r="P54" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>[A4205] PRAED STREET (W2) (Westminster)</t>
-        </is>
-      </c>
-      <c r="R54" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>{'type': 'Point', 'coordinates': [-0.170834, 51.51835], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="T54" t="b">
-        <v>0</v>
-      </c>
-      <c r="U54" t="b">
-        <v>0</v>
-      </c>
-      <c r="V54" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="W54" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="X54" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="Y54" t="inlineStr"/>
-      <c r="Z54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Tfl.Api.Presentation.Entities.RoadDisruption, Tfl.Api.Presentation.Entities</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>TIMS-205512</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>/Road/All/Disruption/TIMS-205512</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>[-0.106039,51.556345]</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Minimal</t>
-        </is>
-      </c>
-      <c r="F55" t="n">
-        <v>54</v>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Planned events</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>Sporting</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>Drayton Park (All approaches) at the junction of Aubert Park - Arsenal v Dynamo Zagreb Football Match.</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Delays possible. </t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>2025-01-22T20:34:23Z</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>2025-01-22T19:00:00Z</t>
-        </is>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>2025-01-22T22:30:00Z</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>2025-01-22T20:34:23Z</t>
-        </is>
-      </c>
-      <c r="P55" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>DRAYTON PARK (N5,N7) (Islington)</t>
-        </is>
-      </c>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>{'type': 'Point', 'coordinates': [-0.106039, 51.556345], 'crs': {'type': 'name', 'properties': {'name': 'EPSG:4326'}}}</t>
-        </is>
-      </c>
-      <c r="T55" t="b">
-        <v>0</v>
-      </c>
-      <c r="U55" t="b">
-        <v>0</v>
-      </c>
-      <c r="V55" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="W55" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="X55" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="Y55" t="inlineStr"/>
-      <c r="Z55" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add weekly archives and automate GitHub Pages deployment
</commit_message>
<xml_diff>
--- a/disruptions.xlsx
+++ b/disruptions.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>